<commit_message>
added logs page in output file
</commit_message>
<xml_diff>
--- a/example1_optcor.xlsx
+++ b/example1_optcor.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Corrected" sheetId="3" r:id="rId5"/>
     <sheet name="Normalized" sheetId="4" r:id="rId6"/>
     <sheet name="PoolAfterDF" sheetId="5" r:id="rId7"/>
+    <sheet name="logs" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="365">
   <si>
     <t>label</t>
   </si>
@@ -368,6 +369,750 @@
   </si>
   <si>
     <t>sample5</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>metaGroupId</t>
+  </si>
+  <si>
+    <t>groupId</t>
+  </si>
+  <si>
+    <t>goodPeakCount</t>
+  </si>
+  <si>
+    <t>medMz</t>
+  </si>
+  <si>
+    <t>medRt</t>
+  </si>
+  <si>
+    <t>maxQuality</t>
+  </si>
+  <si>
+    <t>isotopeLabel</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C13-label-5</t>
+  </si>
+  <si>
+    <t>C13-label-7</t>
+  </si>
+  <si>
+    <t>C13-label-8</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C13-label-6</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-5</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>compoundId</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>C10H16N5O13P3</t>
+  </si>
+  <si>
+    <t>C10H15N5O10P2</t>
+  </si>
+  <si>
+    <t>C10H14N5O7P</t>
+  </si>
+  <si>
+    <t>C3H7NO3</t>
+  </si>
+  <si>
+    <t>C2H5NO2</t>
+  </si>
+  <si>
+    <t>C10H12N4O5</t>
+  </si>
+  <si>
+    <t>C10H14N5O8P</t>
+  </si>
+  <si>
+    <t>expectedRtDiff</t>
+  </si>
+  <si>
+    <t>ppmDiff</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>purity</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>optcorr</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>metaGroupId</t>
+  </si>
+  <si>
+    <t>groupId</t>
+  </si>
+  <si>
+    <t>goodPeakCount</t>
+  </si>
+  <si>
+    <t>medMz</t>
+  </si>
+  <si>
+    <t>medRt</t>
+  </si>
+  <si>
+    <t>maxQuality</t>
+  </si>
+  <si>
+    <t>isotopeLabel</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C13-label-5</t>
+  </si>
+  <si>
+    <t>C13-label-7</t>
+  </si>
+  <si>
+    <t>C13-label-8</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-4</t>
+  </si>
+  <si>
+    <t>C13-label-6</t>
+  </si>
+  <si>
+    <t>C12 PARENT</t>
+  </si>
+  <si>
+    <t>C13-label-1</t>
+  </si>
+  <si>
+    <t>C13-label-2</t>
+  </si>
+  <si>
+    <t>C13-label-3</t>
+  </si>
+  <si>
+    <t>C13-label-5</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>compoundId</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>C10H16N5O13P3</t>
+  </si>
+  <si>
+    <t>C10H15N5O10P2</t>
+  </si>
+  <si>
+    <t>C10H14N5O7P</t>
+  </si>
+  <si>
+    <t>C3H7NO3</t>
+  </si>
+  <si>
+    <t>C2H5NO2</t>
+  </si>
+  <si>
+    <t>C10H12N4O5</t>
+  </si>
+  <si>
+    <t>C10H14N5O8P</t>
+  </si>
+  <si>
+    <t>expectedRtDiff</t>
+  </si>
+  <si>
+    <t>ppmDiff</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>inosine</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>sample5</t>
+  </si>
+  <si>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>purity</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>optcorr</t>
   </si>
 </sst>
 </file>
@@ -388,7 +1133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -400,16 +1145,36 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,61 +1210,61 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>243</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>244</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>245</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>246</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>247</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>248</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>249</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>44</v>
+        <v>286</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>52</v>
+        <v>294</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>60</v>
+        <v>302</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>68</v>
+        <v>310</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>69</v>
+        <v>311</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>70</v>
+        <v>312</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>71</v>
+        <v>313</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>72</v>
+        <v>314</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>73</v>
+        <v>315</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>74</v>
+        <v>316</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>75</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2">
@@ -523,16 +1288,16 @@
         <v>0.85628800000000005</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="L2" s="0">
         <v>0.32000000000000001</v>
@@ -580,16 +1345,16 @@
         <v>0.85578600000000005</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="L3" s="0">
         <v>0.33500000000000002</v>
@@ -637,16 +1402,16 @@
         <v>0.85437300000000005</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>10</v>
+        <v>252</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="L4" s="0">
         <v>0.35599999999999998</v>
@@ -694,16 +1459,16 @@
         <v>0.85048599999999996</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>11</v>
+        <v>253</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="L5" s="0">
         <v>0.34999999999999998</v>
@@ -751,16 +1516,16 @@
         <v>0.136569</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>53</v>
+        <v>295</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="L6" s="0">
         <v>0.38700000000000001</v>
@@ -808,16 +1573,16 @@
         <v>0.81913599999999998</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>54</v>
+        <v>296</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="L7" s="0">
         <v>0.245</v>
@@ -865,16 +1630,16 @@
         <v>0.85572899999999996</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>14</v>
+        <v>256</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>54</v>
+        <v>296</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="L8" s="0">
         <v>0.26200000000000001</v>
@@ -922,16 +1687,16 @@
         <v>0.84935000000000005</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>15</v>
+        <v>257</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>54</v>
+        <v>296</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="L9" s="0">
         <v>0.29699999999999999</v>
@@ -979,16 +1744,16 @@
         <v>0.84013400000000005</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>16</v>
+        <v>258</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>54</v>
+        <v>296</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="L10" s="0">
         <v>0.254</v>
@@ -1036,16 +1801,16 @@
         <v>0.18886700000000001</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>17</v>
+        <v>259</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>54</v>
+        <v>296</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="L11" s="0">
         <v>0.30199999999999999</v>
@@ -1093,16 +1858,16 @@
         <v>0.85546999999999995</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>18</v>
+        <v>260</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L12" s="0">
         <v>0.059999999999999998</v>
@@ -1150,16 +1915,16 @@
         <v>0.85499599999999998</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>19</v>
+        <v>261</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L13" s="0">
         <v>0.057000000000000002</v>
@@ -1207,16 +1972,16 @@
         <v>0.85548800000000003</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>20</v>
+        <v>262</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L14" s="0">
         <v>0.066000000000000003</v>
@@ -1264,16 +2029,16 @@
         <v>0.85197599999999996</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L15" s="0">
         <v>0.071999999999999995</v>
@@ -1321,16 +2086,16 @@
         <v>0.205069</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>22</v>
+        <v>264</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L16" s="0">
         <v>0.050000000000000003</v>
@@ -1378,16 +2143,16 @@
         <v>0.101273</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>23</v>
+        <v>265</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L17" s="0">
         <v>0.067000000000000004</v>
@@ -1435,16 +2200,16 @@
         <v>0.195246</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>24</v>
+        <v>266</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L18" s="0">
         <v>0.068000000000000005</v>
@@ -1492,16 +2257,16 @@
         <v>0.175536</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>25</v>
+        <v>267</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>47</v>
+        <v>289</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>55</v>
+        <v>297</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L19" s="0">
         <v>0.0089999999999999993</v>
@@ -1549,16 +2314,16 @@
         <v>0.84928999999999999</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>26</v>
+        <v>268</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>48</v>
+        <v>290</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>56</v>
+        <v>298</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>64</v>
+        <v>306</v>
       </c>
       <c r="L20" s="0">
         <v>0.057000000000000002</v>
@@ -1606,16 +2371,16 @@
         <v>0.85590500000000003</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>27</v>
+        <v>269</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>48</v>
+        <v>290</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>56</v>
+        <v>298</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>64</v>
+        <v>306</v>
       </c>
       <c r="L21" s="0">
         <v>0.050999999999999997</v>
@@ -1663,16 +2428,16 @@
         <v>0.85286700000000004</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>28</v>
+        <v>270</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>48</v>
+        <v>290</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>56</v>
+        <v>298</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>64</v>
+        <v>306</v>
       </c>
       <c r="L22" s="0">
         <v>0.042000000000000003</v>
@@ -1720,16 +2485,16 @@
         <v>0.85433800000000004</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>29</v>
+        <v>271</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>48</v>
+        <v>290</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>56</v>
+        <v>298</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>64</v>
+        <v>306</v>
       </c>
       <c r="L23" s="0">
         <v>0.064000000000000001</v>
@@ -1777,16 +2542,16 @@
         <v>0.81903000000000004</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>30</v>
+        <v>272</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>49</v>
+        <v>291</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>57</v>
+        <v>299</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="L24" s="0">
         <v>0.074999999999999997</v>
@@ -1834,16 +2599,16 @@
         <v>0.84947600000000001</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>31</v>
+        <v>273</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>49</v>
+        <v>291</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>57</v>
+        <v>299</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="L25" s="0">
         <v>0.066000000000000003</v>
@@ -1891,16 +2656,16 @@
         <v>0.84780999999999995</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>32</v>
+        <v>274</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>49</v>
+        <v>291</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>57</v>
+        <v>299</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>65</v>
+        <v>307</v>
       </c>
       <c r="L26" s="0">
         <v>0.070999999999999994</v>
@@ -1948,16 +2713,16 @@
         <v>0.85062000000000004</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="L27" s="0">
         <v>0.54000000000000004</v>
@@ -2005,16 +2770,16 @@
         <v>0.85219400000000001</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>34</v>
+        <v>276</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="L28" s="0">
         <v>0.52200000000000002</v>
@@ -2062,16 +2827,16 @@
         <v>0.85280900000000004</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>35</v>
+        <v>277</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="L29" s="0">
         <v>0.52100000000000002</v>
@@ -2119,16 +2884,16 @@
         <v>0.85027799999999998</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>36</v>
+        <v>278</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="L30" s="0">
         <v>0.52000000000000002</v>
@@ -2176,16 +2941,16 @@
         <v>0.83695399999999998</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>37</v>
+        <v>279</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="L31" s="0">
         <v>0.52600000000000002</v>
@@ -2233,16 +2998,16 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>38</v>
+        <v>280</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>50</v>
+        <v>292</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="L32" s="0">
         <v>0.52000000000000002</v>
@@ -2290,16 +3055,16 @@
         <v>0.85323499999999997</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>39</v>
+        <v>281</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>51</v>
+        <v>293</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="L33" s="0">
         <v>0.10000000000000001</v>
@@ -2347,16 +3112,16 @@
         <v>0.85544299999999995</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>40</v>
+        <v>282</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>51</v>
+        <v>293</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="L34" s="0">
         <v>0.096000000000000002</v>
@@ -2404,16 +3169,16 @@
         <v>0.85204400000000002</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>41</v>
+        <v>283</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>51</v>
+        <v>293</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="L35" s="0">
         <v>0.097000000000000003</v>
@@ -2461,16 +3226,16 @@
         <v>0.80831799999999998</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>42</v>
+        <v>284</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>51</v>
+        <v>293</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="L36" s="0">
         <v>0.105</v>
@@ -2518,16 +3283,16 @@
         <v>0.31163999999999997</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>43</v>
+        <v>285</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>51</v>
+        <v>293</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="L37" s="0">
         <v>0.051999999999999998</v>
@@ -2565,7 +3330,7 @@
   <cols>
     <col min="1" max="1" width="10.046875" customWidth="true"/>
     <col min="2" max="2" width="5.48828125" customWidth="true"/>
-    <col min="3" max="3" width="14.7109375" customWidth="true"/>
+    <col min="3" max="3" width="15.7109375" customWidth="true"/>
     <col min="4" max="4" width="14.7109375" customWidth="true"/>
     <col min="5" max="5" width="15.7109375" customWidth="true"/>
     <col min="6" max="6" width="15.7109375" customWidth="true"/>
@@ -2574,76 +3339,76 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>76</v>
+        <v>318</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>326</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>327</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>328</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>329</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>330</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>89</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>120257.01773769499</v>
+        <v>119779.8065215385</v>
       </c>
       <c r="D2" s="0">
-        <v>1128175.7858791787</v>
+        <v>1123680.1365549308</v>
       </c>
       <c r="E2" s="0">
-        <v>853856.72753046604</v>
+        <v>850545.61743632285</v>
       </c>
       <c r="F2" s="0">
-        <v>1094755.1716382599</v>
+        <v>1090509.8987583509</v>
       </c>
       <c r="G2" s="0">
-        <v>1124109.8967178694</v>
+        <v>1119607.8997651669</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
       </c>
       <c r="C3" s="0">
-        <v>9032.8924481254544</v>
+        <v>9502.0468962079794</v>
       </c>
       <c r="D3" s="0">
-        <v>77130.716388220579</v>
+        <v>81431.909798725887</v>
       </c>
       <c r="E3" s="0">
-        <v>0.00093724591037384843</v>
+        <v>0.0025544091810980286</v>
       </c>
       <c r="F3" s="0">
-        <v>0.00086344858649177686</v>
+        <v>0.0010672275274116931</v>
       </c>
       <c r="G3" s="0">
-        <v>33792.234279990545</v>
+        <v>38258.936296418091</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B4" s="0">
         <v>2</v>
@@ -2652,21 +3417,21 @@
         <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>0.0017576912038023461</v>
+        <v>0.0016408894887841342</v>
       </c>
       <c r="E4" s="0">
-        <v>0.0005205471606057262</v>
+        <v>0.00047639761305248138</v>
       </c>
       <c r="F4" s="0">
-        <v>0.0008689088389088102</v>
+        <v>0.00072046624547670809</v>
       </c>
       <c r="G4" s="0">
-        <v>0.012277037771535864</v>
+        <v>0.012176759039852936</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B5" s="0">
         <v>3</v>
@@ -2675,7 +3440,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>5970.8198493208602</v>
+        <v>5999.3733711772984</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
@@ -2684,12 +3449,12 @@
         <v>0</v>
       </c>
       <c r="G5" s="0">
-        <v>3558.1123664558454</v>
+        <v>3567.8132330749563</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B6" s="0">
         <v>4</v>
@@ -2712,7 +3477,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B7" s="0">
         <v>5</v>
@@ -2735,7 +3500,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B8" s="0">
         <v>6</v>
@@ -2758,7 +3523,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B9" s="0">
         <v>7</v>
@@ -2781,7 +3546,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B10" s="0">
         <v>8</v>
@@ -2804,7 +3569,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B11" s="0">
         <v>9</v>
@@ -2827,7 +3592,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="B12" s="0">
         <v>10</v>
@@ -2850,76 +3615,76 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>352070.46470118262</v>
+        <v>350723.73739754478</v>
       </c>
       <c r="D13" s="0">
-        <v>3898154.4519998324</v>
+        <v>3882986.272312453</v>
       </c>
       <c r="E13" s="0">
-        <v>3279004.1384339016</v>
+        <v>3264455.6795195448</v>
       </c>
       <c r="F13" s="0">
-        <v>4716223.0711678239</v>
+        <v>4698169.3972747298</v>
       </c>
       <c r="G13" s="0">
-        <v>634319.18584102252</v>
+        <v>631853.13686988922</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
       </c>
       <c r="C14" s="0">
-        <v>25601.926399696313</v>
+        <v>26916.476246369035</v>
       </c>
       <c r="D14" s="0">
-        <v>111322.67703137841</v>
+        <v>126374.11443814464</v>
       </c>
       <c r="E14" s="0">
-        <v>0.066258858418451624</v>
+        <v>10558.556270091169</v>
       </c>
       <c r="F14" s="0">
-        <v>0.0098123546964372782</v>
+        <v>14232.102707285172</v>
       </c>
       <c r="G14" s="0">
-        <v>12551.620729890181</v>
+        <v>15005.398629087194</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B15" s="0">
         <v>2</v>
       </c>
       <c r="C15" s="0">
-        <v>0.0043221054338492973</v>
+        <v>0.00021537993368447706</v>
       </c>
       <c r="D15" s="0">
-        <v>0.062585322283994674</v>
+        <v>0.0031117127640869617</v>
       </c>
       <c r="E15" s="0">
-        <v>3.3128177386208408</v>
+        <v>1974.6127044035645</v>
       </c>
       <c r="F15" s="0">
         <v>0</v>
       </c>
       <c r="G15" s="0">
-        <v>0.0041196491857946292</v>
+        <v>0.0041074793561266167</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B16" s="0">
         <v>3</v>
@@ -2928,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>19525.328332078785</v>
+        <v>19552.827267401408</v>
       </c>
       <c r="E16" s="0">
         <v>0</v>
@@ -2942,7 +3707,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B17" s="0">
         <v>4</v>
@@ -2965,7 +3730,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B18" s="0">
         <v>5</v>
@@ -2988,7 +3753,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B19" s="0">
         <v>6</v>
@@ -3011,7 +3776,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B20" s="0">
         <v>7</v>
@@ -3034,7 +3799,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B21" s="0">
         <v>8</v>
@@ -3057,7 +3822,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B22" s="0">
         <v>9</v>
@@ -3080,7 +3845,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>78</v>
+        <v>320</v>
       </c>
       <c r="B23" s="0">
         <v>10</v>
@@ -3103,88 +3868,88 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B24" s="0">
         <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>19434718.28556272</v>
+        <v>19360496.029138036</v>
       </c>
       <c r="D24" s="0">
-        <v>49405796.55930119</v>
+        <v>49216755.754213199</v>
       </c>
       <c r="E24" s="0">
-        <v>22553096.659726642</v>
+        <v>22464675.73857924</v>
       </c>
       <c r="F24" s="0">
-        <v>26211657.6909809</v>
+        <v>26112332.674518287</v>
       </c>
       <c r="G24" s="0">
-        <v>311768.64371898473</v>
+        <v>310582.42929688597</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B25" s="0">
         <v>1</v>
       </c>
       <c r="C25" s="0">
-        <v>951944.50073897571</v>
+        <v>1022683.3904338363</v>
       </c>
       <c r="D25" s="0">
-        <v>1683763.3845589007</v>
+        <v>1868104.1954691615</v>
       </c>
       <c r="E25" s="0">
-        <v>313917.08566082764</v>
+        <v>399099.80401005951</v>
       </c>
       <c r="F25" s="0">
-        <v>333723.72947626171</v>
+        <v>432463.13616685796</v>
       </c>
       <c r="G25" s="0">
-        <v>17655.093122967501</v>
+        <v>18782.259015639316</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B26" s="0">
         <v>2</v>
       </c>
       <c r="C26" s="0">
-        <v>90269.21197845359</v>
+        <v>93452.733638773279</v>
       </c>
       <c r="D26" s="0">
-        <v>108600.81277102549</v>
+        <v>113290.4473394118</v>
       </c>
       <c r="E26" s="0">
-        <v>96392.905496201187</v>
+        <v>96741.488847717628</v>
       </c>
       <c r="F26" s="0">
-        <v>115971.69091384616</v>
+        <v>116557.2466988245</v>
       </c>
       <c r="G26" s="0">
-        <v>916.49306437842949</v>
+        <v>975.54170894244407</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B27" s="0">
         <v>3</v>
       </c>
       <c r="C27" s="0">
-        <v>31068.626757364891</v>
+        <v>31351.270566664494</v>
       </c>
       <c r="D27" s="0">
-        <v>100161.28640375593</v>
+        <v>104625.00807195068</v>
       </c>
       <c r="E27" s="0">
-        <v>22655.992201474899</v>
+        <v>29815.635537603423</v>
       </c>
       <c r="F27" s="0">
         <v>0</v>
@@ -3195,16 +3960,16 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B28" s="0">
         <v>4</v>
       </c>
       <c r="C28" s="0">
-        <v>798.01533140652089</v>
+        <v>890.57543636706646</v>
       </c>
       <c r="D28" s="0">
-        <v>11675.076532499152</v>
+        <v>15115.44192821202</v>
       </c>
       <c r="E28" s="0">
         <v>0</v>
@@ -3218,7 +3983,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B29" s="0">
         <v>5</v>
@@ -3227,7 +3992,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>13701.009296369981</v>
+        <v>17424.558714710231</v>
       </c>
       <c r="E29" s="0">
         <v>0</v>
@@ -3241,7 +4006,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B30" s="0">
         <v>6</v>
@@ -3250,7 +4015,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>11584.549499348757</v>
+        <v>12440.618780261319</v>
       </c>
       <c r="E30" s="0">
         <v>0</v>
@@ -3264,7 +4029,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B31" s="0">
         <v>7</v>
@@ -3273,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>27442.954025223829</v>
+        <v>31267.468353648233</v>
       </c>
       <c r="E31" s="0">
         <v>0</v>
@@ -3287,7 +4052,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B32" s="0">
         <v>8</v>
@@ -3310,7 +4075,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B33" s="0">
         <v>9</v>
@@ -3333,7 +4098,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="B34" s="0">
         <v>10</v>
@@ -3356,91 +4121,91 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>80</v>
+        <v>322</v>
       </c>
       <c r="B35" s="0">
         <v>0</v>
       </c>
       <c r="C35" s="0">
-        <v>1472555.7146921644</v>
+        <v>1470889.6506570596</v>
       </c>
       <c r="D35" s="0">
-        <v>3452265.1559062968</v>
+        <v>3448359.2847419186</v>
       </c>
       <c r="E35" s="0">
-        <v>2714828.9251858927</v>
+        <v>2711757.3858751352</v>
       </c>
       <c r="F35" s="0">
-        <v>2065530.3058026971</v>
+        <v>2063193.4010297821</v>
       </c>
       <c r="G35" s="0">
-        <v>219793.47220430433</v>
+        <v>219547.32238716495</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>80</v>
+        <v>322</v>
       </c>
       <c r="B36" s="0">
         <v>1</v>
       </c>
       <c r="C36" s="0">
-        <v>81869.348249416362</v>
+        <v>83472.544528304847</v>
       </c>
       <c r="D36" s="0">
-        <v>174683.13008570907</v>
+        <v>178454.81383470277</v>
       </c>
       <c r="E36" s="0">
-        <v>137463.12187956122</v>
+        <v>140428.60661229107</v>
       </c>
       <c r="F36" s="0">
-        <v>98330.408897153771</v>
+        <v>100591.5050919957</v>
       </c>
       <c r="G36" s="0">
-        <v>0.00039211802751877182</v>
+        <v>0.00036893237027482088</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>80</v>
+        <v>322</v>
       </c>
       <c r="B37" s="0">
         <v>2</v>
       </c>
       <c r="C37" s="0">
-        <v>39531.750085368796</v>
+        <v>39578.634294521667</v>
       </c>
       <c r="D37" s="0">
-        <v>66565.156960435066</v>
+        <v>66672.166624857724</v>
       </c>
       <c r="E37" s="0">
-        <v>113512.37534686671</v>
+        <v>113574.5293141719</v>
       </c>
       <c r="F37" s="0">
-        <v>64745.916784606248</v>
+        <v>64796.279960411965</v>
       </c>
       <c r="G37" s="0">
-        <v>2232.9431666787659</v>
+        <v>2242.5492246116846</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>80</v>
+        <v>322</v>
       </c>
       <c r="B38" s="0">
         <v>3</v>
       </c>
       <c r="C38" s="0">
-        <v>75497.586161815416</v>
+        <v>75513.569629731384</v>
       </c>
       <c r="D38" s="0">
-        <v>137428.37542749819</v>
+        <v>137455.55299502725</v>
       </c>
       <c r="E38" s="0">
-        <v>59571.997094997983</v>
+        <v>59615.896767458566</v>
       </c>
       <c r="F38" s="0">
-        <v>63114.858223402247</v>
+        <v>63140.303032550633</v>
       </c>
       <c r="G38" s="0">
         <v>0</v>
@@ -3448,137 +4213,137 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>81</v>
+        <v>323</v>
       </c>
       <c r="B39" s="0">
         <v>0</v>
       </c>
       <c r="C39" s="0">
-        <v>4991337.219774453</v>
+        <v>4987581.577684354</v>
       </c>
       <c r="D39" s="0">
-        <v>9945458.2149231434</v>
+        <v>9938019.1954551656</v>
       </c>
       <c r="E39" s="0">
-        <v>8529328.3909843732</v>
+        <v>8522895.5577582866</v>
       </c>
       <c r="F39" s="0">
-        <v>9828455.9295988064</v>
+        <v>9821043.2588145174</v>
       </c>
       <c r="G39" s="0">
-        <v>687896.23770371522</v>
+        <v>687382.61609358399</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>81</v>
+        <v>323</v>
       </c>
       <c r="B40" s="0">
         <v>1</v>
       </c>
       <c r="C40" s="0">
-        <v>0.0080952013688442553</v>
+        <v>2883.3634078899022</v>
       </c>
       <c r="D40" s="0">
-        <v>0.28462495716763864</v>
+        <v>1318.9318187955598</v>
       </c>
       <c r="E40" s="0">
-        <v>22317.137761748461</v>
+        <v>28737.810333987964</v>
       </c>
       <c r="F40" s="0">
-        <v>34605.113044262798</v>
+        <v>41999.972896705389</v>
       </c>
       <c r="G40" s="0">
-        <v>0.00060300573964683921</v>
+        <v>0.00055504706716487677</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>81</v>
+        <v>323</v>
       </c>
       <c r="B41" s="0">
         <v>2</v>
       </c>
       <c r="C41" s="0">
-        <v>234154.97506496275</v>
+        <v>234184.46819632303</v>
       </c>
       <c r="D41" s="0">
-        <v>333947.90963459498</v>
+        <v>334141.81957947789</v>
       </c>
       <c r="E41" s="0">
-        <v>335731.92863915436</v>
+        <v>335744.09282334434</v>
       </c>
       <c r="F41" s="0">
-        <v>445422.3262861938</v>
+        <v>445440.13664909446</v>
       </c>
       <c r="G41" s="0">
-        <v>19023.634776587096</v>
+        <v>19039.775674804168</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B42" s="0">
         <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>12893969.50967221</v>
+        <v>12845338.748159776</v>
       </c>
       <c r="D42" s="0">
-        <v>13996531.422253933</v>
+        <v>13943737.443609221</v>
       </c>
       <c r="E42" s="0">
-        <v>4723056.7964469474</v>
+        <v>4705246.1402883362</v>
       </c>
       <c r="F42" s="0">
-        <v>4968109.4291885579</v>
+        <v>4949375.6231914507</v>
       </c>
       <c r="G42" s="0">
-        <v>101159.8290401423</v>
+        <v>100779.55714388097</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B43" s="0">
         <v>1</v>
       </c>
       <c r="C43" s="0">
-        <v>298072.94008210371</v>
+        <v>345566.99112924031</v>
       </c>
       <c r="D43" s="0">
-        <v>348872.4397214799</v>
+        <v>400341.6261069157</v>
       </c>
       <c r="E43" s="0">
-        <v>59455.96490358247</v>
+        <v>77021.807693453724</v>
       </c>
       <c r="F43" s="0">
-        <v>49300.243670436932</v>
+        <v>67857.744706191908</v>
       </c>
       <c r="G43" s="0">
-        <v>3284.7517074235334</v>
+        <v>3658.8818047999357</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B44" s="0">
         <v>2</v>
       </c>
       <c r="C44" s="0">
-        <v>74133.701532528561</v>
+        <v>74999.556059812749</v>
       </c>
       <c r="D44" s="0">
-        <v>87354.912772026262</v>
+        <v>88360.670747944707</v>
       </c>
       <c r="E44" s="0">
-        <v>15932.559119754045</v>
+        <v>16115.443816756231</v>
       </c>
       <c r="F44" s="0">
-        <v>6974.9477452975552</v>
+        <v>6833.8184042828761</v>
       </c>
       <c r="G44" s="0">
         <v>0</v>
@@ -3586,22 +4351,22 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B45" s="0">
         <v>3</v>
       </c>
       <c r="C45" s="0">
-        <v>30261.595826901408</v>
+        <v>30465.808357167611</v>
       </c>
       <c r="D45" s="0">
-        <v>26497.251492526018</v>
+        <v>26743.277550742656</v>
       </c>
       <c r="E45" s="0">
-        <v>609.4089893760156</v>
+        <v>671.3371279443578</v>
       </c>
       <c r="F45" s="0">
-        <v>1268.2992742119716</v>
+        <v>1346.6060867557619</v>
       </c>
       <c r="G45" s="0">
         <v>0</v>
@@ -3609,16 +4374,16 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B46" s="0">
         <v>4</v>
       </c>
       <c r="C46" s="0">
-        <v>0.0015693815837089216</v>
+        <v>0.0014131746154544341</v>
       </c>
       <c r="D46" s="0">
-        <v>107.2388215207166</v>
+        <v>180.25214987162849</v>
       </c>
       <c r="E46" s="0">
         <v>0</v>
@@ -3632,13 +4397,13 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B47" s="0">
         <v>5</v>
       </c>
       <c r="C47" s="0">
-        <v>0.03148377990336277</v>
+        <v>0.028348490794686706</v>
       </c>
       <c r="D47" s="0">
         <v>0</v>
@@ -3655,13 +4420,13 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B48" s="0">
         <v>6</v>
       </c>
       <c r="C48" s="0">
-        <v>1037.1641327884249</v>
+        <v>1036.1493690692346</v>
       </c>
       <c r="D48" s="0">
         <v>0</v>
@@ -3678,7 +4443,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B49" s="0">
         <v>7</v>
@@ -3701,7 +4466,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B50" s="0">
         <v>8</v>
@@ -3724,7 +4489,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B51" s="0">
         <v>9</v>
@@ -3747,7 +4512,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B52" s="0">
         <v>10</v>
@@ -3770,68 +4535,68 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
       </c>
       <c r="C53" s="0">
-        <v>1537477.7039064453</v>
+        <v>1531192.3788513434</v>
       </c>
       <c r="D53" s="0">
-        <v>5963499.2094822563</v>
+        <v>5940993.1259224275</v>
       </c>
       <c r="E53" s="0">
-        <v>1623048.2719497499</v>
+        <v>1616865.1867830809</v>
       </c>
       <c r="F53" s="0">
-        <v>1975516.2594665675</v>
+        <v>1968703.2035333083</v>
       </c>
       <c r="G53" s="0">
-        <v>136712.36705407614</v>
+        <v>136240.88053633319</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B54" s="0">
         <v>1</v>
       </c>
       <c r="C54" s="0">
-        <v>44061.288841223424</v>
+        <v>49780.383008635014</v>
       </c>
       <c r="D54" s="0">
-        <v>78054.429362902461</v>
+        <v>98163.628517867153</v>
       </c>
       <c r="E54" s="0">
-        <v>14307.911983946464</v>
+        <v>20054.923952503676</v>
       </c>
       <c r="F54" s="0">
-        <v>0.00096703172245735038</v>
+        <v>0.00090161239855469357</v>
       </c>
       <c r="G54" s="0">
-        <v>0.00020200463860172449</v>
+        <v>0.00018932359567083127</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B55" s="0">
         <v>2</v>
       </c>
       <c r="C55" s="0">
-        <v>8305.4726959470318</v>
+        <v>8423.02676804164</v>
       </c>
       <c r="D55" s="0">
-        <v>24730.041605600622</v>
+        <v>25124.501031331631</v>
       </c>
       <c r="E55" s="0">
-        <v>7476.4555512059887</v>
+        <v>7529.1031784423476</v>
       </c>
       <c r="F55" s="0">
-        <v>0.048419612769699</v>
+        <v>0.046164774577961309</v>
       </c>
       <c r="G55" s="0">
         <v>0</v>
@@ -3839,16 +4604,16 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B56" s="0">
         <v>3</v>
       </c>
       <c r="C56" s="0">
-        <v>679.55892751680176</v>
+        <v>1174.9860433012277</v>
       </c>
       <c r="D56" s="0">
-        <v>5291.0903048251557</v>
+        <v>4770.6656043711037</v>
       </c>
       <c r="E56" s="0">
         <v>0</v>
@@ -3862,13 +4627,13 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B57" s="0">
         <v>4</v>
       </c>
       <c r="C57" s="0">
-        <v>137.09644357228174</v>
+        <v>89.398186954837769</v>
       </c>
       <c r="D57" s="0">
         <v>0</v>
@@ -3885,13 +4650,13 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B58" s="0">
         <v>5</v>
       </c>
       <c r="C58" s="0">
-        <v>1418.3877203092122</v>
+        <v>1414.3998755580949</v>
       </c>
       <c r="D58" s="0">
         <v>0</v>
@@ -3908,7 +4673,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B59" s="0">
         <v>6</v>
@@ -3931,7 +4696,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B60" s="0">
         <v>7</v>
@@ -3954,7 +4719,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B61" s="0">
         <v>8</v>
@@ -3977,7 +4742,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B62" s="0">
         <v>9</v>
@@ -4000,7 +4765,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="B63" s="0">
         <v>10</v>
@@ -4041,39 +4806,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>90</v>
+        <v>332</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>98</v>
+        <v>340</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>99</v>
+        <v>341</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>100</v>
+        <v>342</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>101</v>
+        <v>343</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>102</v>
+        <v>344</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>103</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>0.93013000000000001</v>
+        <v>0.92649999999999999</v>
       </c>
       <c r="D2" s="0">
-        <v>0.93139000000000005</v>
+        <v>0.92779999999999996</v>
       </c>
       <c r="E2" s="0">
         <v>0.99999000000000005</v>
@@ -4082,21 +4847,21 @@
         <v>0.99999000000000005</v>
       </c>
       <c r="G2" s="0">
-        <v>0.96784000000000003</v>
+        <v>0.96397999999999995</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
       </c>
       <c r="C3" s="0">
-        <v>0.069860000000000005</v>
+        <v>0.07349</v>
       </c>
       <c r="D3" s="0">
-        <v>0.063670000000000004</v>
+        <v>0.067229999999999998</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
@@ -4105,12 +4870,12 @@
         <v>0</v>
       </c>
       <c r="G3" s="0">
-        <v>0.029090000000000001</v>
+        <v>0.032939999999999997</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B4" s="0">
         <v>2</v>
@@ -4133,7 +4898,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B5" s="0">
         <v>3</v>
@@ -4142,7 +4907,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>0.0049199999999999999</v>
+        <v>0.0049500000000000004</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
@@ -4151,12 +4916,12 @@
         <v>0</v>
       </c>
       <c r="G5" s="0">
-        <v>0.0030599999999999998</v>
+        <v>0.0030699999999999998</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B6" s="0">
         <v>4</v>
@@ -4179,7 +4944,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B7" s="0">
         <v>5</v>
@@ -4202,7 +4967,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B8" s="0">
         <v>6</v>
@@ -4225,7 +4990,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B9" s="0">
         <v>7</v>
@@ -4248,7 +5013,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B10" s="0">
         <v>8</v>
@@ -4271,7 +5036,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B11" s="0">
         <v>9</v>
@@ -4294,7 +5059,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>91</v>
+        <v>333</v>
       </c>
       <c r="B12" s="0">
         <v>10</v>
@@ -4317,53 +5082,53 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>0.93220999999999998</v>
+        <v>0.92871999999999999</v>
       </c>
       <c r="D13" s="0">
-        <v>0.96752000000000005</v>
+        <v>0.96377999999999997</v>
       </c>
       <c r="E13" s="0">
-        <v>0.99999000000000005</v>
+        <v>0.99617</v>
       </c>
       <c r="F13" s="0">
-        <v>0.99999000000000005</v>
+        <v>0.99697000000000002</v>
       </c>
       <c r="G13" s="0">
-        <v>0.98058999999999996</v>
+        <v>0.9768</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
       </c>
       <c r="C14" s="0">
-        <v>0.067780000000000007</v>
+        <v>0.07127</v>
       </c>
       <c r="D14" s="0">
-        <v>0.027629999999999998</v>
+        <v>0.031359999999999999</v>
       </c>
       <c r="E14" s="0">
-        <v>0</v>
+        <v>0.0032200000000000002</v>
       </c>
       <c r="F14" s="0">
-        <v>0</v>
+        <v>0.0030200000000000001</v>
       </c>
       <c r="G14" s="0">
-        <v>0.019400000000000001</v>
+        <v>0.023189999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B15" s="0">
         <v>2</v>
@@ -4375,7 +5140,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="0">
-        <v>0</v>
+        <v>0.00059999999999999995</v>
       </c>
       <c r="F15" s="0">
         <v>0</v>
@@ -4386,7 +5151,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B16" s="0">
         <v>3</v>
@@ -4395,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>0.0048399999999999997</v>
+        <v>0.0048500000000000001</v>
       </c>
       <c r="E16" s="0">
         <v>0</v>
@@ -4409,7 +5174,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B17" s="0">
         <v>4</v>
@@ -4432,7 +5197,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B18" s="0">
         <v>5</v>
@@ -4455,7 +5220,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B19" s="0">
         <v>6</v>
@@ -4478,7 +5243,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B20" s="0">
         <v>7</v>
@@ -4501,7 +5266,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B21" s="0">
         <v>8</v>
@@ -4524,7 +5289,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B22" s="0">
         <v>9</v>
@@ -4547,7 +5312,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>92</v>
+        <v>334</v>
       </c>
       <c r="B23" s="0">
         <v>10</v>
@@ -4570,88 +5335,88 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B24" s="0">
         <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>0.94762000000000002</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="D24" s="0">
-        <v>0.96189000000000002</v>
+        <v>0.95791000000000004</v>
       </c>
       <c r="E24" s="0">
-        <v>0.98116000000000003</v>
+        <v>0.97713000000000005</v>
       </c>
       <c r="F24" s="0">
-        <v>0.98312999999999995</v>
+        <v>0.97940000000000005</v>
       </c>
       <c r="G24" s="0">
-        <v>0.94377999999999995</v>
+        <v>0.94018000000000002</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B25" s="0">
         <v>1</v>
       </c>
       <c r="C25" s="0">
-        <v>0.04641</v>
+        <v>0.049860000000000002</v>
       </c>
       <c r="D25" s="0">
-        <v>0.032779999999999997</v>
+        <v>0.03635</v>
       </c>
       <c r="E25" s="0">
-        <v>0.013650000000000001</v>
+        <v>0.017350000000000001</v>
       </c>
       <c r="F25" s="0">
-        <v>0.01251</v>
+        <v>0.016219999999999998</v>
       </c>
       <c r="G25" s="0">
-        <v>0.053440000000000001</v>
+        <v>0.056849999999999998</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B26" s="0">
         <v>2</v>
       </c>
       <c r="C26" s="0">
-        <v>0.0044000000000000003</v>
+        <v>0.0045500000000000002</v>
       </c>
       <c r="D26" s="0">
-        <v>0.0021099999999999999</v>
+        <v>0.0022000000000000001</v>
       </c>
       <c r="E26" s="0">
-        <v>0.0041900000000000001</v>
+        <v>0.0041999999999999997</v>
       </c>
       <c r="F26" s="0">
-        <v>0.0043400000000000001</v>
+        <v>0.0043699999999999998</v>
       </c>
       <c r="G26" s="0">
-        <v>0.0027699999999999999</v>
+        <v>0.0029499999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B27" s="0">
         <v>3</v>
       </c>
       <c r="C27" s="0">
-        <v>0.0015100000000000001</v>
+        <v>0.0015200000000000001</v>
       </c>
       <c r="D27" s="0">
-        <v>0.0019499999999999999</v>
+        <v>0.0020300000000000001</v>
       </c>
       <c r="E27" s="0">
-        <v>0.00097999999999999997</v>
+        <v>0.0012899999999999999</v>
       </c>
       <c r="F27" s="0">
         <v>0</v>
@@ -4662,16 +5427,16 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B28" s="0">
         <v>4</v>
       </c>
       <c r="C28" s="0">
-        <v>3.0000000000000001e-05</v>
+        <v>4.0000000000000003e-05</v>
       </c>
       <c r="D28" s="0">
-        <v>0.00022000000000000001</v>
+        <v>0.00029</v>
       </c>
       <c r="E28" s="0">
         <v>0</v>
@@ -4685,7 +5450,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B29" s="0">
         <v>5</v>
@@ -4694,7 +5459,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>0.00025999999999999998</v>
+        <v>0.00033</v>
       </c>
       <c r="E29" s="0">
         <v>0</v>
@@ -4708,7 +5473,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B30" s="0">
         <v>6</v>
@@ -4717,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>0.00022000000000000001</v>
+        <v>0.00024000000000000001</v>
       </c>
       <c r="E30" s="0">
         <v>0</v>
@@ -4731,7 +5496,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B31" s="0">
         <v>7</v>
@@ -4740,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>0.00052999999999999998</v>
+        <v>0.00059999999999999995</v>
       </c>
       <c r="E31" s="0">
         <v>0</v>
@@ -4754,7 +5519,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B32" s="0">
         <v>8</v>
@@ -4777,7 +5542,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B33" s="0">
         <v>9</v>
@@ -4800,7 +5565,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="B34" s="0">
         <v>10</v>
@@ -4823,45 +5588,45 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>94</v>
+        <v>336</v>
       </c>
       <c r="B35" s="0">
         <v>0</v>
       </c>
       <c r="C35" s="0">
-        <v>0.88205</v>
+        <v>0.88105999999999995</v>
       </c>
       <c r="D35" s="0">
-        <v>0.90115000000000001</v>
+        <v>0.90012999999999999</v>
       </c>
       <c r="E35" s="0">
-        <v>0.89734999999999998</v>
+        <v>0.89632999999999996</v>
       </c>
       <c r="F35" s="0">
-        <v>0.90129999999999999</v>
+        <v>0.90027999999999997</v>
       </c>
       <c r="G35" s="0">
-        <v>0.98994000000000004</v>
+        <v>0.98987999999999998</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>94</v>
+        <v>336</v>
       </c>
       <c r="B36" s="0">
         <v>1</v>
       </c>
       <c r="C36" s="0">
-        <v>0.049029999999999997</v>
+        <v>0.04999</v>
       </c>
       <c r="D36" s="0">
-        <v>0.045589999999999999</v>
+        <v>0.046580000000000003</v>
       </c>
       <c r="E36" s="0">
-        <v>0.045429999999999998</v>
+        <v>0.04641</v>
       </c>
       <c r="F36" s="0">
-        <v>0.042900000000000001</v>
+        <v>0.043889999999999998</v>
       </c>
       <c r="G36" s="0">
         <v>0</v>
@@ -4869,45 +5634,45 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>94</v>
+        <v>336</v>
       </c>
       <c r="B37" s="0">
         <v>2</v>
       </c>
       <c r="C37" s="0">
-        <v>0.02367</v>
+        <v>0.023699999999999999</v>
       </c>
       <c r="D37" s="0">
-        <v>0.01737</v>
+        <v>0.017399999999999999</v>
       </c>
       <c r="E37" s="0">
-        <v>0.037519999999999998</v>
+        <v>0.037539999999999997</v>
       </c>
       <c r="F37" s="0">
-        <v>0.028250000000000001</v>
+        <v>0.02827</v>
       </c>
       <c r="G37" s="0">
-        <v>0.01005</v>
+        <v>0.010109999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>94</v>
+        <v>336</v>
       </c>
       <c r="B38" s="0">
         <v>3</v>
       </c>
       <c r="C38" s="0">
-        <v>0.045220000000000003</v>
+        <v>0.045229999999999999</v>
       </c>
       <c r="D38" s="0">
-        <v>0.035869999999999999</v>
+        <v>0.035880000000000002</v>
       </c>
       <c r="E38" s="0">
-        <v>0.019689999999999999</v>
+        <v>0.019699999999999999</v>
       </c>
       <c r="F38" s="0">
-        <v>0.027539999999999999</v>
+        <v>0.027550000000000002</v>
       </c>
       <c r="G38" s="0">
         <v>0</v>
@@ -4915,45 +5680,45 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>95</v>
+        <v>337</v>
       </c>
       <c r="B39" s="0">
         <v>0</v>
       </c>
       <c r="C39" s="0">
-        <v>0.95518000000000003</v>
+        <v>0.95462000000000002</v>
       </c>
       <c r="D39" s="0">
-        <v>0.96750999999999998</v>
+        <v>0.96733999999999998</v>
       </c>
       <c r="E39" s="0">
-        <v>0.95970999999999995</v>
+        <v>0.95898000000000005</v>
       </c>
       <c r="F39" s="0">
-        <v>0.95343</v>
+        <v>0.95270999999999995</v>
       </c>
       <c r="G39" s="0">
-        <v>0.97307999999999995</v>
+        <v>0.97304000000000002</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>95</v>
+        <v>337</v>
       </c>
       <c r="B40" s="0">
         <v>1</v>
       </c>
       <c r="C40" s="0">
-        <v>0</v>
+        <v>0.00055000000000000003</v>
       </c>
       <c r="D40" s="0">
-        <v>0</v>
+        <v>0.00012</v>
       </c>
       <c r="E40" s="0">
-        <v>0.0025100000000000001</v>
+        <v>0.0032299999999999998</v>
       </c>
       <c r="F40" s="0">
-        <v>0.0033500000000000001</v>
+        <v>0.0040699999999999998</v>
       </c>
       <c r="G40" s="0">
         <v>0</v>
@@ -4961,91 +5726,91 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>95</v>
+        <v>337</v>
       </c>
       <c r="B41" s="0">
         <v>2</v>
       </c>
       <c r="C41" s="0">
-        <v>0.044810000000000003</v>
+        <v>0.044819999999999999</v>
       </c>
       <c r="D41" s="0">
-        <v>0.032480000000000002</v>
+        <v>0.03252</v>
       </c>
       <c r="E41" s="0">
         <v>0.037769999999999998</v>
       </c>
       <c r="F41" s="0">
-        <v>0.043200000000000002</v>
+        <v>0.043209999999999998</v>
       </c>
       <c r="G41" s="0">
-        <v>0.02691</v>
+        <v>0.026950000000000002</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B42" s="0">
         <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>0.96965000000000001</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="D42" s="0">
-        <v>0.96799000000000002</v>
+        <v>0.96433000000000002</v>
       </c>
       <c r="E42" s="0">
-        <v>0.98416000000000003</v>
+        <v>0.98045000000000004</v>
       </c>
       <c r="F42" s="0">
-        <v>0.98855000000000004</v>
+        <v>0.98485999999999996</v>
       </c>
       <c r="G42" s="0">
-        <v>0.96855000000000002</v>
+        <v>0.96496000000000004</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B43" s="0">
         <v>1</v>
       </c>
       <c r="C43" s="0">
-        <v>0.022409999999999999</v>
+        <v>0.02598</v>
       </c>
       <c r="D43" s="0">
-        <v>0.024119999999999999</v>
+        <v>0.02768</v>
       </c>
       <c r="E43" s="0">
-        <v>0.01238</v>
+        <v>0.016039999999999999</v>
       </c>
       <c r="F43" s="0">
-        <v>0.0097999999999999997</v>
+        <v>0.0135</v>
       </c>
       <c r="G43" s="0">
-        <v>0.031440000000000003</v>
+        <v>0.035029999999999999</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B44" s="0">
         <v>2</v>
       </c>
       <c r="C44" s="0">
-        <v>0.0055700000000000003</v>
+        <v>0.00564</v>
       </c>
       <c r="D44" s="0">
-        <v>0.0060400000000000002</v>
+        <v>0.00611</v>
       </c>
       <c r="E44" s="0">
-        <v>0.00331</v>
+        <v>0.0033500000000000001</v>
       </c>
       <c r="F44" s="0">
-        <v>0.0013799999999999999</v>
+        <v>0.0013500000000000001</v>
       </c>
       <c r="G44" s="0">
         <v>0</v>
@@ -5053,22 +5818,22 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B45" s="0">
         <v>3</v>
       </c>
       <c r="C45" s="0">
-        <v>0.0022699999999999999</v>
+        <v>0.0022899999999999999</v>
       </c>
       <c r="D45" s="0">
-        <v>0.00183</v>
+        <v>0.0018400000000000001</v>
       </c>
       <c r="E45" s="0">
-        <v>0.00012</v>
+        <v>0.00012999999999999999</v>
       </c>
       <c r="F45" s="0">
-        <v>0.00025000000000000001</v>
+        <v>0.00025999999999999998</v>
       </c>
       <c r="G45" s="0">
         <v>0</v>
@@ -5076,7 +5841,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B46" s="0">
         <v>4</v>
@@ -5085,7 +5850,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="0">
-        <v>0</v>
+        <v>1.0000000000000001e-05</v>
       </c>
       <c r="E46" s="0">
         <v>0</v>
@@ -5099,7 +5864,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B47" s="0">
         <v>5</v>
@@ -5122,7 +5887,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B48" s="0">
         <v>6</v>
@@ -5145,7 +5910,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B49" s="0">
         <v>7</v>
@@ -5168,7 +5933,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B50" s="0">
         <v>8</v>
@@ -5191,7 +5956,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B51" s="0">
         <v>9</v>
@@ -5214,7 +5979,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="B52" s="0">
         <v>10</v>
@@ -5237,19 +6002,19 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
       </c>
       <c r="C53" s="0">
-        <v>0.9657</v>
+        <v>0.96174999999999999</v>
       </c>
       <c r="D53" s="0">
-        <v>0.98219000000000001</v>
+        <v>0.97889000000000004</v>
       </c>
       <c r="E53" s="0">
-        <v>0.98675000000000002</v>
+        <v>0.98321999999999998</v>
       </c>
       <c r="F53" s="0">
         <v>0.99999000000000005</v>
@@ -5260,19 +6025,19 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B54" s="0">
         <v>1</v>
       </c>
       <c r="C54" s="0">
-        <v>0.02767</v>
+        <v>0.031260000000000003</v>
       </c>
       <c r="D54" s="0">
-        <v>0.01285</v>
+        <v>0.01617</v>
       </c>
       <c r="E54" s="0">
-        <v>0.0086899999999999998</v>
+        <v>0.012189999999999999</v>
       </c>
       <c r="F54" s="0">
         <v>0</v>
@@ -5283,19 +6048,19 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B55" s="0">
         <v>2</v>
       </c>
       <c r="C55" s="0">
-        <v>0.0052100000000000002</v>
+        <v>0.0052900000000000004</v>
       </c>
       <c r="D55" s="0">
-        <v>0.0040699999999999998</v>
+        <v>0.00413</v>
       </c>
       <c r="E55" s="0">
-        <v>0.0045399999999999998</v>
+        <v>0.0045700000000000003</v>
       </c>
       <c r="F55" s="0">
         <v>0</v>
@@ -5306,16 +6071,16 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B56" s="0">
         <v>3</v>
       </c>
       <c r="C56" s="0">
-        <v>0.00042000000000000002</v>
+        <v>0.00072999999999999996</v>
       </c>
       <c r="D56" s="0">
-        <v>0.00087000000000000001</v>
+        <v>0.00077999999999999999</v>
       </c>
       <c r="E56" s="0">
         <v>0</v>
@@ -5329,13 +6094,13 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B57" s="0">
         <v>4</v>
       </c>
       <c r="C57" s="0">
-        <v>8.0000000000000007e-05</v>
+        <v>5.0000000000000002e-05</v>
       </c>
       <c r="D57" s="0">
         <v>0</v>
@@ -5352,13 +6117,13 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B58" s="0">
         <v>5</v>
       </c>
       <c r="C58" s="0">
-        <v>0.00088999999999999995</v>
+        <v>0.00088000000000000003</v>
       </c>
       <c r="D58" s="0">
         <v>0</v>
@@ -5375,7 +6140,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B59" s="0">
         <v>6</v>
@@ -5398,7 +6163,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B60" s="0">
         <v>7</v>
@@ -5421,7 +6186,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B61" s="0">
         <v>8</v>
@@ -5444,7 +6209,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B62" s="0">
         <v>9</v>
@@ -5467,7 +6232,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="B63" s="0">
         <v>10</v>
@@ -5507,27 +6272,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>104</v>
+        <v>346</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>112</v>
+        <v>354</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>113</v>
+        <v>355</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>114</v>
+        <v>356</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>115</v>
+        <v>357</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>116</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>105</v>
+        <v>347</v>
       </c>
       <c r="B2" s="0">
         <v>125187.68000000001</v>
@@ -5547,7 +6312,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>106</v>
+        <v>348</v>
       </c>
       <c r="B3" s="0">
         <v>372516.72999999998</v>
@@ -5567,7 +6332,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>107</v>
+        <v>349</v>
       </c>
       <c r="B4" s="0">
         <v>20507084.09</v>
@@ -5587,7 +6352,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>108</v>
+        <v>350</v>
       </c>
       <c r="B5" s="0">
         <v>1669454.4000000001</v>
@@ -5607,7 +6372,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>109</v>
+        <v>351</v>
       </c>
       <c r="B6" s="0">
         <v>5224649.4099999992</v>
@@ -5627,7 +6392,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>110</v>
+        <v>352</v>
       </c>
       <c r="B7" s="0">
         <v>13296737.390000002</v>
@@ -5647,7 +6412,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>111</v>
+        <v>353</v>
       </c>
       <c r="B8" s="0">
         <v>1593925.8099999998</v>
@@ -5663,6 +6428,67 @@
       </c>
       <c r="F8" s="0">
         <v>128836.13</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.37890625" customWidth="true"/>
+    <col min="2" max="2" width="7.26953125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.98999999999999999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3" s="0">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" s="0">
+        <v>211.32060970000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="0">
+        <v>211.85279370000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
computational speed up 3X
auto adjust mzWindow and stepsize for gaussian peak convolution, speed up by 3X
</commit_message>
<xml_diff>
--- a/example1_optcor.xlsx
+++ b/example1_optcor.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxing\Documents\Github\optCorr_script\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D4C511-F9AB-412A-B4E4-AA727DB5F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="528" yWindow="852" windowWidth="20892" windowHeight="11136" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Original" sheetId="2" r:id="rId3"/>
-    <sheet name="Corrected" sheetId="3" r:id="rId5"/>
-    <sheet name="Normalized" sheetId="4" r:id="rId6"/>
-    <sheet name="PoolAfterDF" sheetId="5" r:id="rId7"/>
-    <sheet name="logs" sheetId="6" r:id="rId8"/>
+    <sheet name="Original" sheetId="2" r:id="rId1"/>
+    <sheet name="Corrected" sheetId="3" r:id="rId2"/>
+    <sheet name="Normalized" sheetId="4" r:id="rId3"/>
+    <sheet name="PoolAfterDF" sheetId="5" r:id="rId4"/>
+    <sheet name="logs" sheetId="6" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="246">
   <si>
     <t>label</t>
   </si>
@@ -371,360 +377,6 @@
     <t>sample5</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>metaGroupId</t>
-  </si>
-  <si>
-    <t>groupId</t>
-  </si>
-  <si>
-    <t>goodPeakCount</t>
-  </si>
-  <si>
-    <t>medMz</t>
-  </si>
-  <si>
-    <t>medRt</t>
-  </si>
-  <si>
-    <t>maxQuality</t>
-  </si>
-  <si>
-    <t>isotopeLabel</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C13-label-3</t>
-  </si>
-  <si>
-    <t>C13-label-4</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C13-label-3</t>
-  </si>
-  <si>
-    <t>C13-label-4</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C13-label-3</t>
-  </si>
-  <si>
-    <t>C13-label-4</t>
-  </si>
-  <si>
-    <t>C13-label-5</t>
-  </si>
-  <si>
-    <t>C13-label-7</t>
-  </si>
-  <si>
-    <t>C13-label-8</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C13-label-3</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C13-label-3</t>
-  </si>
-  <si>
-    <t>C13-label-4</t>
-  </si>
-  <si>
-    <t>C13-label-6</t>
-  </si>
-  <si>
-    <t>C12 PARENT</t>
-  </si>
-  <si>
-    <t>C13-label-1</t>
-  </si>
-  <si>
-    <t>C13-label-2</t>
-  </si>
-  <si>
-    <t>C13-label-3</t>
-  </si>
-  <si>
-    <t>C13-label-5</t>
-  </si>
-  <si>
-    <t>compound</t>
-  </si>
-  <si>
-    <t>ATP</t>
-  </si>
-  <si>
-    <t>ADP</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
-    <t>serine</t>
-  </si>
-  <si>
-    <t>glycine</t>
-  </si>
-  <si>
-    <t>inosine</t>
-  </si>
-  <si>
-    <t>GMP</t>
-  </si>
-  <si>
-    <t>compoundId</t>
-  </si>
-  <si>
-    <t>ATP</t>
-  </si>
-  <si>
-    <t>ADP</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
-    <t>serine</t>
-  </si>
-  <si>
-    <t>glycine</t>
-  </si>
-  <si>
-    <t>inosine</t>
-  </si>
-  <si>
-    <t>GMP</t>
-  </si>
-  <si>
-    <t>formula</t>
-  </si>
-  <si>
-    <t>C10H16N5O13P3</t>
-  </si>
-  <si>
-    <t>C10H15N5O10P2</t>
-  </si>
-  <si>
-    <t>C10H14N5O7P</t>
-  </si>
-  <si>
-    <t>C3H7NO3</t>
-  </si>
-  <si>
-    <t>C2H5NO2</t>
-  </si>
-  <si>
-    <t>C10H12N4O5</t>
-  </si>
-  <si>
-    <t>C10H14N5O8P</t>
-  </si>
-  <si>
-    <t>expectedRtDiff</t>
-  </si>
-  <si>
-    <t>ppmDiff</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sample4</t>
-  </si>
-  <si>
-    <t>sample5</t>
-  </si>
-  <si>
-    <t>Compound</t>
-  </si>
-  <si>
-    <t>ATP</t>
-  </si>
-  <si>
-    <t>ADP</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
-    <t>serine</t>
-  </si>
-  <si>
-    <t>glycine</t>
-  </si>
-  <si>
-    <t>inosine</t>
-  </si>
-  <si>
-    <t>GMP</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sample4</t>
-  </si>
-  <si>
-    <t>sample5</t>
-  </si>
-  <si>
-    <t>Compound</t>
-  </si>
-  <si>
-    <t>ATP</t>
-  </si>
-  <si>
-    <t>ADP</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
-    <t>serine</t>
-  </si>
-  <si>
-    <t>glycine</t>
-  </si>
-  <si>
-    <t>inosine</t>
-  </si>
-  <si>
-    <t>GMP</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sample4</t>
-  </si>
-  <si>
-    <t>sample5</t>
-  </si>
-  <si>
-    <t>Compound</t>
-  </si>
-  <si>
-    <t>ATP</t>
-  </si>
-  <si>
-    <t>ADP</t>
-  </si>
-  <si>
-    <t>AMP</t>
-  </si>
-  <si>
-    <t>serine</t>
-  </si>
-  <si>
-    <t>glycine</t>
-  </si>
-  <si>
-    <t>inosine</t>
-  </si>
-  <si>
-    <t>GMP</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sample4</t>
-  </si>
-  <si>
-    <t>sample5</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>solver</t>
   </si>
   <si>
@@ -738,9 +390,6 @@
   </si>
   <si>
     <t>runtime</t>
-  </si>
-  <si>
-    <t>C2</t>
   </si>
   <si>
     <t>optcorr</t>
@@ -1118,7 +767,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -1133,7 +782,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1146,46 +795,336 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S37"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5.046875" customWidth="true"/>
     <col min="2" max="2" width="11.93359375" customWidth="true"/>
@@ -1201,70 +1140,70 @@
     <col min="12" max="12" width="13.37890625" customWidth="true"/>
     <col min="13" max="13" width="8.7109375" customWidth="true"/>
     <col min="14" max="14" width="10.7109375" customWidth="true"/>
+    <col min="18" max="18" width="9.7109375" customWidth="true"/>
     <col min="15" max="15" width="10.7109375" customWidth="true"/>
     <col min="16" max="16" width="10.7109375" customWidth="true"/>
     <col min="17" max="17" width="10.7109375" customWidth="true"/>
-    <col min="18" max="18" width="9.7109375" customWidth="true"/>
     <col min="19" max="19" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>242</v>
+        <v>123</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>243</v>
+        <v>124</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>245</v>
+        <v>126</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>246</v>
+        <v>127</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>247</v>
+        <v>128</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>248</v>
+        <v>129</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>249</v>
+        <v>130</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>286</v>
+        <v>167</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>294</v>
+        <v>175</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>302</v>
+        <v>183</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>310</v>
+        <v>191</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>311</v>
+        <v>192</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>312</v>
+        <v>193</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>313</v>
+        <v>194</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>314</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>315</v>
+        <v>196</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>316</v>
+        <v>197</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>317</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2">
@@ -1288,16 +1227,16 @@
         <v>0.85628800000000005</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>250</v>
+        <v>131</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>295</v>
+        <v>176</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="L2" s="0">
         <v>0.32000000000000001</v>
@@ -1345,16 +1284,16 @@
         <v>0.85578600000000005</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>251</v>
+        <v>132</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>295</v>
+        <v>176</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="L3" s="0">
         <v>0.33500000000000002</v>
@@ -1402,16 +1341,16 @@
         <v>0.85437300000000005</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>252</v>
+        <v>133</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>295</v>
+        <v>176</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="L4" s="0">
         <v>0.35599999999999998</v>
@@ -1459,16 +1398,16 @@
         <v>0.85048599999999996</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>253</v>
+        <v>134</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>295</v>
+        <v>176</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="L5" s="0">
         <v>0.34999999999999998</v>
@@ -1516,16 +1455,16 @@
         <v>0.136569</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>254</v>
+        <v>135</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>295</v>
+        <v>176</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="L6" s="0">
         <v>0.38700000000000001</v>
@@ -1573,16 +1512,16 @@
         <v>0.81913599999999998</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>255</v>
+        <v>136</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>288</v>
+        <v>169</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>296</v>
+        <v>177</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>304</v>
+        <v>185</v>
       </c>
       <c r="L7" s="0">
         <v>0.245</v>
@@ -1630,16 +1569,16 @@
         <v>0.85572899999999996</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>256</v>
+        <v>137</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>288</v>
+        <v>169</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>296</v>
+        <v>177</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>304</v>
+        <v>185</v>
       </c>
       <c r="L8" s="0">
         <v>0.26200000000000001</v>
@@ -1687,16 +1626,16 @@
         <v>0.84935000000000005</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>257</v>
+        <v>138</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>288</v>
+        <v>169</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>296</v>
+        <v>177</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>304</v>
+        <v>185</v>
       </c>
       <c r="L9" s="0">
         <v>0.29699999999999999</v>
@@ -1744,16 +1683,16 @@
         <v>0.84013400000000005</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>258</v>
+        <v>139</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>288</v>
+        <v>169</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>296</v>
+        <v>177</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>304</v>
+        <v>185</v>
       </c>
       <c r="L10" s="0">
         <v>0.254</v>
@@ -1801,16 +1740,16 @@
         <v>0.18886700000000001</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>259</v>
+        <v>140</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>288</v>
+        <v>169</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>296</v>
+        <v>177</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>304</v>
+        <v>185</v>
       </c>
       <c r="L11" s="0">
         <v>0.30199999999999999</v>
@@ -1858,16 +1797,16 @@
         <v>0.85546999999999995</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>260</v>
+        <v>141</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L12" s="0">
         <v>0.059999999999999998</v>
@@ -1915,16 +1854,16 @@
         <v>0.85499599999999998</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>261</v>
+        <v>142</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L13" s="0">
         <v>0.057000000000000002</v>
@@ -1972,16 +1911,16 @@
         <v>0.85548800000000003</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>262</v>
+        <v>143</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L14" s="0">
         <v>0.066000000000000003</v>
@@ -2029,16 +1968,16 @@
         <v>0.85197599999999996</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>263</v>
+        <v>144</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L15" s="0">
         <v>0.071999999999999995</v>
@@ -2086,16 +2025,16 @@
         <v>0.205069</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>264</v>
+        <v>145</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L16" s="0">
         <v>0.050000000000000003</v>
@@ -2143,16 +2082,16 @@
         <v>0.101273</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>265</v>
+        <v>146</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L17" s="0">
         <v>0.067000000000000004</v>
@@ -2200,16 +2139,16 @@
         <v>0.195246</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>266</v>
+        <v>147</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L18" s="0">
         <v>0.068000000000000005</v>
@@ -2257,16 +2196,16 @@
         <v>0.175536</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>289</v>
+        <v>170</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>305</v>
+        <v>186</v>
       </c>
       <c r="L19" s="0">
         <v>0.0089999999999999993</v>
@@ -2314,16 +2253,16 @@
         <v>0.84928999999999999</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>268</v>
+        <v>149</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>290</v>
+        <v>171</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>298</v>
+        <v>179</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>306</v>
+        <v>187</v>
       </c>
       <c r="L20" s="0">
         <v>0.057000000000000002</v>
@@ -2371,16 +2310,16 @@
         <v>0.85590500000000003</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>269</v>
+        <v>150</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>290</v>
+        <v>171</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>298</v>
+        <v>179</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>306</v>
+        <v>187</v>
       </c>
       <c r="L21" s="0">
         <v>0.050999999999999997</v>
@@ -2428,16 +2367,16 @@
         <v>0.85286700000000004</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>270</v>
+        <v>151</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>290</v>
+        <v>171</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>298</v>
+        <v>179</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>306</v>
+        <v>187</v>
       </c>
       <c r="L22" s="0">
         <v>0.042000000000000003</v>
@@ -2485,16 +2424,16 @@
         <v>0.85433800000000004</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>271</v>
+        <v>152</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>290</v>
+        <v>171</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>298</v>
+        <v>179</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>306</v>
+        <v>187</v>
       </c>
       <c r="L23" s="0">
         <v>0.064000000000000001</v>
@@ -2542,16 +2481,16 @@
         <v>0.81903000000000004</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>272</v>
+        <v>153</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>291</v>
+        <v>172</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>299</v>
+        <v>180</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="L24" s="0">
         <v>0.074999999999999997</v>
@@ -2599,16 +2538,16 @@
         <v>0.84947600000000001</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>273</v>
+        <v>154</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>291</v>
+        <v>172</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>299</v>
+        <v>180</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="L25" s="0">
         <v>0.066000000000000003</v>
@@ -2656,16 +2595,16 @@
         <v>0.84780999999999995</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>274</v>
+        <v>155</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>291</v>
+        <v>172</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>299</v>
+        <v>180</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="L26" s="0">
         <v>0.070999999999999994</v>
@@ -2713,16 +2652,16 @@
         <v>0.85062000000000004</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>275</v>
+        <v>156</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>300</v>
+        <v>181</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="L27" s="0">
         <v>0.54000000000000004</v>
@@ -2770,16 +2709,16 @@
         <v>0.85219400000000001</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>276</v>
+        <v>157</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>300</v>
+        <v>181</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="L28" s="0">
         <v>0.52200000000000002</v>
@@ -2827,16 +2766,16 @@
         <v>0.85280900000000004</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>277</v>
+        <v>158</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>300</v>
+        <v>181</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="L29" s="0">
         <v>0.52100000000000002</v>
@@ -2884,16 +2823,16 @@
         <v>0.85027799999999998</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>278</v>
+        <v>159</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>300</v>
+        <v>181</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="L30" s="0">
         <v>0.52000000000000002</v>
@@ -2941,16 +2880,16 @@
         <v>0.83695399999999998</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>279</v>
+        <v>160</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>300</v>
+        <v>181</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="L31" s="0">
         <v>0.52600000000000002</v>
@@ -2998,16 +2937,16 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>280</v>
+        <v>161</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>292</v>
+        <v>173</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>300</v>
+        <v>181</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>308</v>
+        <v>189</v>
       </c>
       <c r="L32" s="0">
         <v>0.52000000000000002</v>
@@ -3055,16 +2994,16 @@
         <v>0.85323499999999997</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>281</v>
+        <v>162</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>293</v>
+        <v>174</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>301</v>
+        <v>182</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="L33" s="0">
         <v>0.10000000000000001</v>
@@ -3112,16 +3051,16 @@
         <v>0.85544299999999995</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>282</v>
+        <v>163</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>293</v>
+        <v>174</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>301</v>
+        <v>182</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="L34" s="0">
         <v>0.096000000000000002</v>
@@ -3169,16 +3108,16 @@
         <v>0.85204400000000002</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>283</v>
+        <v>164</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>293</v>
+        <v>174</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>301</v>
+        <v>182</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="L35" s="0">
         <v>0.097000000000000003</v>
@@ -3226,16 +3165,16 @@
         <v>0.80831799999999998</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>284</v>
+        <v>165</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>293</v>
+        <v>174</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>301</v>
+        <v>182</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="L36" s="0">
         <v>0.105</v>
@@ -3283,16 +3222,16 @@
         <v>0.31163999999999997</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>285</v>
+        <v>166</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>293</v>
+        <v>174</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>301</v>
+        <v>182</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>309</v>
+        <v>190</v>
       </c>
       <c r="L37" s="0">
         <v>0.051999999999999998</v>
@@ -3320,95 +3259,99 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G63"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.046875" customWidth="true"/>
     <col min="2" max="2" width="5.48828125" customWidth="true"/>
     <col min="3" max="3" width="15.7109375" customWidth="true"/>
     <col min="4" max="4" width="14.7109375" customWidth="true"/>
-    <col min="5" max="5" width="15.7109375" customWidth="true"/>
     <col min="6" max="6" width="15.7109375" customWidth="true"/>
     <col min="7" max="7" width="15.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>318</v>
+        <v>199</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>326</v>
+        <v>207</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>327</v>
+        <v>208</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>328</v>
+        <v>209</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>329</v>
+        <v>210</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>330</v>
+        <v>211</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>331</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>119779.8065215385</v>
+        <v>119779.55453865761</v>
       </c>
       <c r="D2" s="0">
-        <v>1123680.1365549308</v>
+        <v>1123676.9368395088</v>
       </c>
       <c r="E2" s="0">
-        <v>850545.61743632285</v>
+        <v>850542.80264220573</v>
       </c>
       <c r="F2" s="0">
-        <v>1090509.8987583509</v>
+        <v>1090506.2898268157</v>
       </c>
       <c r="G2" s="0">
-        <v>1119607.8997651669</v>
+        <v>1119604.1579320682</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
       </c>
       <c r="C3" s="0">
-        <v>9502.0468962079794</v>
+        <v>9501.7211219054789</v>
       </c>
       <c r="D3" s="0">
-        <v>81431.909798725887</v>
+        <v>81435.611458094834</v>
       </c>
       <c r="E3" s="0">
-        <v>0.0025544091810980286</v>
+        <v>0.0025497205896362167</v>
       </c>
       <c r="F3" s="0">
-        <v>0.0010672275274116931</v>
+        <v>0.0010666579583756993</v>
       </c>
       <c r="G3" s="0">
-        <v>38258.936296418091</v>
+        <v>38262.570299333791</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B4" s="0">
         <v>2</v>
@@ -3417,21 +3360,21 @@
         <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>0.0016408894887841342</v>
+        <v>0.0016488799184973255</v>
       </c>
       <c r="E4" s="0">
-        <v>0.00047639761305248138</v>
+        <v>0.0004731021207341193</v>
       </c>
       <c r="F4" s="0">
-        <v>0.00072046624547670809</v>
+        <v>0.00071546412595058348</v>
       </c>
       <c r="G4" s="0">
-        <v>0.012176759039852936</v>
+        <v>0.0006083532809313427</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B5" s="0">
         <v>3</v>
@@ -3440,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>5999.3733711772984</v>
+        <v>5999.5907255317425</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
@@ -3449,12 +3392,12 @@
         <v>0</v>
       </c>
       <c r="G5" s="0">
-        <v>3567.8132330749563</v>
+        <v>3567.9080584218282</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B6" s="0">
         <v>4</v>
@@ -3477,7 +3420,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B7" s="0">
         <v>5</v>
@@ -3500,7 +3443,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B8" s="0">
         <v>6</v>
@@ -3523,7 +3466,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B9" s="0">
         <v>7</v>
@@ -3546,7 +3489,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B10" s="0">
         <v>8</v>
@@ -3569,7 +3512,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B11" s="0">
         <v>9</v>
@@ -3592,7 +3535,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="B12" s="0">
         <v>10</v>
@@ -3615,76 +3558,76 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>350723.73739754478</v>
+        <v>350722.7084846028</v>
       </c>
       <c r="D13" s="0">
-        <v>3882986.272312453</v>
+        <v>3882980.9134806893</v>
       </c>
       <c r="E13" s="0">
-        <v>3264455.6795195448</v>
+        <v>3264885.465580327</v>
       </c>
       <c r="F13" s="0">
-        <v>4698169.3972747298</v>
+        <v>4698170.4027480641</v>
       </c>
       <c r="G13" s="0">
-        <v>631853.13686988922</v>
+        <v>631852.7287012462</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
       </c>
       <c r="C14" s="0">
-        <v>26916.476246369035</v>
+        <v>26916.429982662521</v>
       </c>
       <c r="D14" s="0">
-        <v>126374.11443814464</v>
+        <v>126408.01689949643</v>
       </c>
       <c r="E14" s="0">
-        <v>10558.556270091169</v>
+        <v>10567.985748494446</v>
       </c>
       <c r="F14" s="0">
-        <v>14232.102707285172</v>
+        <v>14231.097242824335</v>
       </c>
       <c r="G14" s="0">
-        <v>15005.398629087194</v>
+        <v>15007.050599441518</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B15" s="0">
         <v>2</v>
       </c>
       <c r="C15" s="0">
-        <v>0.00021537993368447706</v>
+        <v>0.00021475526995120127</v>
       </c>
       <c r="D15" s="0">
-        <v>0.0031117127640869617</v>
+        <v>0.062658309810676507</v>
       </c>
       <c r="E15" s="0">
-        <v>1974.6127044035645</v>
+        <v>1535.3966777033399</v>
       </c>
       <c r="F15" s="0">
         <v>0</v>
       </c>
       <c r="G15" s="0">
-        <v>0.0041074793561266167</v>
+        <v>0.0041317102854733318</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B16" s="0">
         <v>3</v>
@@ -3693,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>19552.827267401408</v>
+        <v>19559.292925023801</v>
       </c>
       <c r="E16" s="0">
         <v>0</v>
@@ -3707,7 +3650,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B17" s="0">
         <v>4</v>
@@ -3730,7 +3673,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B18" s="0">
         <v>5</v>
@@ -3753,7 +3696,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B19" s="0">
         <v>6</v>
@@ -3776,7 +3719,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B20" s="0">
         <v>7</v>
@@ -3799,7 +3742,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B21" s="0">
         <v>8</v>
@@ -3822,7 +3765,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B22" s="0">
         <v>9</v>
@@ -3845,7 +3788,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>320</v>
+        <v>201</v>
       </c>
       <c r="B23" s="0">
         <v>10</v>
@@ -3868,88 +3811,88 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B24" s="0">
         <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>19360496.029138036</v>
+        <v>19360459.802760698</v>
       </c>
       <c r="D24" s="0">
-        <v>49216755.754213199</v>
+        <v>49217827.706196919</v>
       </c>
       <c r="E24" s="0">
-        <v>22464675.73857924</v>
+        <v>22465166.613843944</v>
       </c>
       <c r="F24" s="0">
-        <v>26112332.674518287</v>
+        <v>26113357.210149404</v>
       </c>
       <c r="G24" s="0">
-        <v>310582.42929688597</v>
+        <v>310997.81842794712</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B25" s="0">
         <v>1</v>
       </c>
       <c r="C25" s="0">
-        <v>1022683.3904338363</v>
+        <v>1022754.1289526828</v>
       </c>
       <c r="D25" s="0">
-        <v>1868104.1954691615</v>
+        <v>1866366.4511449237</v>
       </c>
       <c r="E25" s="0">
-        <v>399099.80401005951</v>
+        <v>398759.6246068168</v>
       </c>
       <c r="F25" s="0">
-        <v>432463.13616685796</v>
+        <v>432528.01005094801</v>
       </c>
       <c r="G25" s="0">
-        <v>18782.259015639316</v>
+        <v>19148.55568367675</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B26" s="0">
         <v>2</v>
       </c>
       <c r="C26" s="0">
-        <v>93452.733638773279</v>
+        <v>93437.922041073311</v>
       </c>
       <c r="D26" s="0">
-        <v>113290.4473394118</v>
+        <v>111480.43841085707</v>
       </c>
       <c r="E26" s="0">
-        <v>96741.488847717628</v>
+        <v>95852.544804576828</v>
       </c>
       <c r="F26" s="0">
-        <v>116557.2466988245</v>
+        <v>115467.8607575257</v>
       </c>
       <c r="G26" s="0">
-        <v>975.54170894244407</v>
+        <v>2.6959129896764988</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B27" s="0">
         <v>3</v>
       </c>
       <c r="C27" s="0">
-        <v>31351.270566664494</v>
+        <v>31293.501998232274</v>
       </c>
       <c r="D27" s="0">
-        <v>104625.00807195068</v>
+        <v>103342.55513592529</v>
       </c>
       <c r="E27" s="0">
-        <v>29815.635537603423</v>
+        <v>29660.027777881282</v>
       </c>
       <c r="F27" s="0">
         <v>0</v>
@@ -3960,16 +3903,16 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B28" s="0">
         <v>4</v>
       </c>
       <c r="C28" s="0">
-        <v>890.57543636706646</v>
+        <v>886.7027930912468</v>
       </c>
       <c r="D28" s="0">
-        <v>15115.44192821202</v>
+        <v>13865.16315013924</v>
       </c>
       <c r="E28" s="0">
         <v>0</v>
@@ -3983,7 +3926,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B29" s="0">
         <v>5</v>
@@ -3992,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>17424.558714710231</v>
+        <v>14785.754948354121</v>
       </c>
       <c r="E29" s="0">
         <v>0</v>
@@ -4006,7 +3949,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B30" s="0">
         <v>6</v>
@@ -4015,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>12440.618780261319</v>
+        <v>11313.079526479656</v>
       </c>
       <c r="E30" s="0">
         <v>0</v>
@@ -4029,7 +3972,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B31" s="0">
         <v>7</v>
@@ -4038,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>31267.468353648233</v>
+        <v>30094.076055342488</v>
       </c>
       <c r="E31" s="0">
         <v>0</v>
@@ -4052,7 +3995,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B32" s="0">
         <v>8</v>
@@ -4075,7 +4018,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B33" s="0">
         <v>9</v>
@@ -4098,7 +4041,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>321</v>
+        <v>202</v>
       </c>
       <c r="B34" s="0">
         <v>10</v>
@@ -4121,7 +4064,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>322</v>
+        <v>203</v>
       </c>
       <c r="B35" s="0">
         <v>0</v>
@@ -4139,12 +4082,12 @@
         <v>2063193.4010297821</v>
       </c>
       <c r="G35" s="0">
-        <v>219547.32238716495</v>
+        <v>219547.32274970226</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>322</v>
+        <v>203</v>
       </c>
       <c r="B36" s="0">
         <v>1</v>
@@ -4162,12 +4105,12 @@
         <v>100591.5050919957</v>
       </c>
       <c r="G36" s="0">
-        <v>0.00036893237027482088</v>
+        <v>0.00036893242301841499</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>322</v>
+        <v>203</v>
       </c>
       <c r="B37" s="0">
         <v>2</v>
@@ -4185,12 +4128,12 @@
         <v>64796.279960411965</v>
       </c>
       <c r="G37" s="0">
-        <v>2242.5492246116846</v>
+        <v>2242.5467267080658</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>322</v>
+        <v>203</v>
       </c>
       <c r="B38" s="0">
         <v>3</v>
@@ -4213,7 +4156,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>323</v>
+        <v>204</v>
       </c>
       <c r="B39" s="0">
         <v>0</v>
@@ -4236,7 +4179,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>323</v>
+        <v>204</v>
       </c>
       <c r="B40" s="0">
         <v>1</v>
@@ -4259,7 +4202,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>323</v>
+        <v>204</v>
       </c>
       <c r="B41" s="0">
         <v>2</v>
@@ -4282,68 +4225,68 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B42" s="0">
         <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>12845338.748159776</v>
+        <v>12845285.705434522</v>
       </c>
       <c r="D42" s="0">
-        <v>13943737.443609221</v>
+        <v>13943681.188013986</v>
       </c>
       <c r="E42" s="0">
-        <v>4705246.1402883362</v>
+        <v>4705228.3479185961</v>
       </c>
       <c r="F42" s="0">
-        <v>4949375.6231914507</v>
+        <v>4949357.4855928998</v>
       </c>
       <c r="G42" s="0">
-        <v>100779.55714388097</v>
+        <v>100779.19532526248</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B43" s="0">
         <v>1</v>
       </c>
       <c r="C43" s="0">
-        <v>345566.99112924031</v>
+        <v>345625.84890830028</v>
       </c>
       <c r="D43" s="0">
-        <v>400341.6261069157</v>
+        <v>400404.00907547108</v>
       </c>
       <c r="E43" s="0">
-        <v>77021.807693453724</v>
+        <v>77041.445933195952</v>
       </c>
       <c r="F43" s="0">
-        <v>67857.744706191908</v>
+        <v>67879.117765748946</v>
       </c>
       <c r="G43" s="0">
-        <v>3658.8818047999357</v>
+        <v>3659.2399065848335</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B44" s="0">
         <v>2</v>
       </c>
       <c r="C44" s="0">
-        <v>74999.556059812749</v>
+        <v>74993.664624276396</v>
       </c>
       <c r="D44" s="0">
-        <v>88360.670747944707</v>
+        <v>88354.17696893336</v>
       </c>
       <c r="E44" s="0">
-        <v>16115.443816756231</v>
+        <v>16113.541303250362</v>
       </c>
       <c r="F44" s="0">
-        <v>6833.8184042828761</v>
+        <v>7023.0107585757787</v>
       </c>
       <c r="G44" s="0">
         <v>0</v>
@@ -4351,22 +4294,22 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B45" s="0">
         <v>3</v>
       </c>
       <c r="C45" s="0">
-        <v>30465.808357167611</v>
+        <v>30465.878743230471</v>
       </c>
       <c r="D45" s="0">
-        <v>26743.277550742656</v>
+        <v>26743.668841800318</v>
       </c>
       <c r="E45" s="0">
-        <v>671.3371279443578</v>
+        <v>671.39498495342843</v>
       </c>
       <c r="F45" s="0">
-        <v>1346.6060867557619</v>
+        <v>1330.0892435090295</v>
       </c>
       <c r="G45" s="0">
         <v>0</v>
@@ -4374,16 +4317,16 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B46" s="0">
         <v>4</v>
       </c>
       <c r="C46" s="0">
-        <v>0.0014131746154544341</v>
+        <v>0.00035343484626798469</v>
       </c>
       <c r="D46" s="0">
-        <v>180.25214987162849</v>
+        <v>180.23407544629609</v>
       </c>
       <c r="E46" s="0">
         <v>0</v>
@@ -4397,13 +4340,13 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B47" s="0">
         <v>5</v>
       </c>
       <c r="C47" s="0">
-        <v>0.028348490794686706</v>
+        <v>0.0070899716266002374</v>
       </c>
       <c r="D47" s="0">
         <v>0</v>
@@ -4420,13 +4363,13 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B48" s="0">
         <v>6</v>
       </c>
       <c r="C48" s="0">
-        <v>1036.1493690692346</v>
+        <v>1036.1452937845063</v>
       </c>
       <c r="D48" s="0">
         <v>0</v>
@@ -4443,7 +4386,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B49" s="0">
         <v>7</v>
@@ -4466,7 +4409,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B50" s="0">
         <v>8</v>
@@ -4489,7 +4432,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B51" s="0">
         <v>9</v>
@@ -4512,7 +4455,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>324</v>
+        <v>205</v>
       </c>
       <c r="B52" s="0">
         <v>10</v>
@@ -4535,68 +4478,68 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
       </c>
       <c r="C53" s="0">
-        <v>1531192.3788513434</v>
+        <v>1531227.3924099074</v>
       </c>
       <c r="D53" s="0">
-        <v>5940993.1259224275</v>
+        <v>5941150.050775555</v>
       </c>
       <c r="E53" s="0">
-        <v>1616865.1867830809</v>
+        <v>1616915.0068290958</v>
       </c>
       <c r="F53" s="0">
-        <v>1968703.2035333083</v>
+        <v>1968703.936385399</v>
       </c>
       <c r="G53" s="0">
-        <v>136240.88053633319</v>
+        <v>136240.93152764239</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B54" s="0">
         <v>1</v>
       </c>
       <c r="C54" s="0">
-        <v>49780.383008635014</v>
+        <v>49783.396328016206</v>
       </c>
       <c r="D54" s="0">
-        <v>98163.628517867153</v>
+        <v>98058.168787793562</v>
       </c>
       <c r="E54" s="0">
-        <v>20054.923952503676</v>
+        <v>20296.3734248252</v>
       </c>
       <c r="F54" s="0">
-        <v>0.00090161239855469357</v>
+        <v>0.00090019689242448557</v>
       </c>
       <c r="G54" s="0">
-        <v>0.00018932359567083127</v>
+        <v>0.00018931549438157562</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B55" s="0">
         <v>2</v>
       </c>
       <c r="C55" s="0">
-        <v>8423.02676804164</v>
+        <v>8423.3889893919059</v>
       </c>
       <c r="D55" s="0">
-        <v>25124.501031331631</v>
+        <v>24780.469265080861</v>
       </c>
       <c r="E55" s="0">
-        <v>7529.1031784423476</v>
+        <v>7409.301681752293</v>
       </c>
       <c r="F55" s="0">
-        <v>0.046164774577961309</v>
+        <v>0.050218643370856603</v>
       </c>
       <c r="G55" s="0">
         <v>0</v>
@@ -4604,16 +4547,16 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B56" s="0">
         <v>3</v>
       </c>
       <c r="C56" s="0">
-        <v>1174.9860433012277</v>
+        <v>1162.8299220547849</v>
       </c>
       <c r="D56" s="0">
-        <v>4770.6656043711037</v>
+        <v>4814.4993678188175</v>
       </c>
       <c r="E56" s="0">
         <v>0</v>
@@ -4627,13 +4570,13 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B57" s="0">
         <v>4</v>
       </c>
       <c r="C57" s="0">
-        <v>89.398186954837769</v>
+        <v>61.137881585123708</v>
       </c>
       <c r="D57" s="0">
         <v>0</v>
@@ -4650,13 +4593,13 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B58" s="0">
         <v>5</v>
       </c>
       <c r="C58" s="0">
-        <v>1414.3998755580949</v>
+        <v>1416.3714314046331</v>
       </c>
       <c r="D58" s="0">
         <v>0</v>
@@ -4673,7 +4616,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B59" s="0">
         <v>6</v>
@@ -4696,7 +4639,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B60" s="0">
         <v>7</v>
@@ -4719,7 +4662,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B61" s="0">
         <v>8</v>
@@ -4742,7 +4685,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B62" s="0">
         <v>9</v>
@@ -4765,7 +4708,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>325</v>
+        <v>206</v>
       </c>
       <c r="B63" s="0">
         <v>10</v>
@@ -4787,13 +4730,17 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G63"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.046875" customWidth="true"/>
     <col min="2" max="2" width="5.48828125" customWidth="true"/>
@@ -4806,30 +4753,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>332</v>
+        <v>213</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>340</v>
+        <v>221</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>341</v>
+        <v>222</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>342</v>
+        <v>223</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>343</v>
+        <v>224</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>344</v>
+        <v>225</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>345</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -4852,7 +4799,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
@@ -4861,7 +4808,7 @@
         <v>0.07349</v>
       </c>
       <c r="D3" s="0">
-        <v>0.067229999999999998</v>
+        <v>0.067239999999999994</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
@@ -4875,7 +4822,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B4" s="0">
         <v>2</v>
@@ -4898,7 +4845,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B5" s="0">
         <v>3</v>
@@ -4921,7 +4868,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B6" s="0">
         <v>4</v>
@@ -4944,7 +4891,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B7" s="0">
         <v>5</v>
@@ -4967,7 +4914,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B8" s="0">
         <v>6</v>
@@ -4990,7 +4937,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B9" s="0">
         <v>7</v>
@@ -5013,7 +4960,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B10" s="0">
         <v>8</v>
@@ -5036,7 +4983,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B11" s="0">
         <v>9</v>
@@ -5059,7 +5006,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>333</v>
+        <v>214</v>
       </c>
       <c r="B12" s="0">
         <v>10</v>
@@ -5082,7 +5029,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
@@ -5091,13 +5038,13 @@
         <v>0.92871999999999999</v>
       </c>
       <c r="D13" s="0">
-        <v>0.96377999999999997</v>
+        <v>0.96377000000000002</v>
       </c>
       <c r="E13" s="0">
-        <v>0.99617</v>
+        <v>0.99629999999999996</v>
       </c>
       <c r="F13" s="0">
-        <v>0.99697000000000002</v>
+        <v>0.99697999999999998</v>
       </c>
       <c r="G13" s="0">
         <v>0.9768</v>
@@ -5105,7 +5052,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B14" s="0">
         <v>1</v>
@@ -5114,13 +5061,13 @@
         <v>0.07127</v>
       </c>
       <c r="D14" s="0">
-        <v>0.031359999999999999</v>
+        <v>0.031370000000000002</v>
       </c>
       <c r="E14" s="0">
         <v>0.0032200000000000002</v>
       </c>
       <c r="F14" s="0">
-        <v>0.0030200000000000001</v>
+        <v>0.0030100000000000001</v>
       </c>
       <c r="G14" s="0">
         <v>0.023189999999999999</v>
@@ -5128,7 +5075,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B15" s="0">
         <v>2</v>
@@ -5140,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="0">
-        <v>0.00059999999999999995</v>
+        <v>0.00046000000000000001</v>
       </c>
       <c r="F15" s="0">
         <v>0</v>
@@ -5151,7 +5098,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B16" s="0">
         <v>3</v>
@@ -5174,7 +5121,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B17" s="0">
         <v>4</v>
@@ -5197,7 +5144,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B18" s="0">
         <v>5</v>
@@ -5220,7 +5167,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B19" s="0">
         <v>6</v>
@@ -5243,7 +5190,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B20" s="0">
         <v>7</v>
@@ -5266,7 +5213,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B21" s="0">
         <v>8</v>
@@ -5289,7 +5236,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B22" s="0">
         <v>9</v>
@@ -5312,7 +5259,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="B23" s="0">
         <v>10</v>
@@ -5335,7 +5282,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B24" s="0">
         <v>0</v>
@@ -5344,21 +5291,21 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="D24" s="0">
-        <v>0.95791000000000004</v>
+        <v>0.95811999999999997</v>
       </c>
       <c r="E24" s="0">
-        <v>0.97713000000000005</v>
+        <v>0.97719</v>
       </c>
       <c r="F24" s="0">
-        <v>0.97940000000000005</v>
+        <v>0.97943999999999998</v>
       </c>
       <c r="G24" s="0">
-        <v>0.94018000000000002</v>
+        <v>0.94198999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B25" s="0">
         <v>1</v>
@@ -5367,21 +5314,21 @@
         <v>0.049860000000000002</v>
       </c>
       <c r="D25" s="0">
-        <v>0.03635</v>
+        <v>0.036330000000000001</v>
       </c>
       <c r="E25" s="0">
-        <v>0.017350000000000001</v>
+        <v>0.017340000000000001</v>
       </c>
       <c r="F25" s="0">
         <v>0.016219999999999998</v>
       </c>
       <c r="G25" s="0">
-        <v>0.056849999999999998</v>
+        <v>0.05799</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B26" s="0">
         <v>2</v>
@@ -5390,21 +5337,21 @@
         <v>0.0045500000000000002</v>
       </c>
       <c r="D26" s="0">
-        <v>0.0022000000000000001</v>
+        <v>0.0021700000000000001</v>
       </c>
       <c r="E26" s="0">
-        <v>0.0041999999999999997</v>
+        <v>0.0041599999999999996</v>
       </c>
       <c r="F26" s="0">
-        <v>0.0043699999999999998</v>
+        <v>0.0043299999999999996</v>
       </c>
       <c r="G26" s="0">
-        <v>0.0029499999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B27" s="0">
         <v>3</v>
@@ -5413,7 +5360,7 @@
         <v>0.0015200000000000001</v>
       </c>
       <c r="D27" s="0">
-        <v>0.0020300000000000001</v>
+        <v>0.0020100000000000001</v>
       </c>
       <c r="E27" s="0">
         <v>0.0012899999999999999</v>
@@ -5427,7 +5374,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B28" s="0">
         <v>4</v>
@@ -5436,7 +5383,7 @@
         <v>4.0000000000000003e-05</v>
       </c>
       <c r="D28" s="0">
-        <v>0.00029</v>
+        <v>0.00025999999999999998</v>
       </c>
       <c r="E28" s="0">
         <v>0</v>
@@ -5450,7 +5397,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B29" s="0">
         <v>5</v>
@@ -5459,7 +5406,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>0.00033</v>
+        <v>0.00027999999999999998</v>
       </c>
       <c r="E29" s="0">
         <v>0</v>
@@ -5473,7 +5420,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B30" s="0">
         <v>6</v>
@@ -5482,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>0.00024000000000000001</v>
+        <v>0.00022000000000000001</v>
       </c>
       <c r="E30" s="0">
         <v>0</v>
@@ -5496,7 +5443,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B31" s="0">
         <v>7</v>
@@ -5505,7 +5452,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>0.00059999999999999995</v>
+        <v>0.00058</v>
       </c>
       <c r="E31" s="0">
         <v>0</v>
@@ -5519,7 +5466,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B32" s="0">
         <v>8</v>
@@ -5542,7 +5489,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B33" s="0">
         <v>9</v>
@@ -5565,7 +5512,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>335</v>
+        <v>216</v>
       </c>
       <c r="B34" s="0">
         <v>10</v>
@@ -5588,7 +5535,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>336</v>
+        <v>217</v>
       </c>
       <c r="B35" s="0">
         <v>0</v>
@@ -5611,7 +5558,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>336</v>
+        <v>217</v>
       </c>
       <c r="B36" s="0">
         <v>1</v>
@@ -5634,7 +5581,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>336</v>
+        <v>217</v>
       </c>
       <c r="B37" s="0">
         <v>2</v>
@@ -5657,7 +5604,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>336</v>
+        <v>217</v>
       </c>
       <c r="B38" s="0">
         <v>3</v>
@@ -5680,7 +5627,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>337</v>
+        <v>218</v>
       </c>
       <c r="B39" s="0">
         <v>0</v>
@@ -5703,7 +5650,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>337</v>
+        <v>218</v>
       </c>
       <c r="B40" s="0">
         <v>1</v>
@@ -5726,7 +5673,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>337</v>
+        <v>218</v>
       </c>
       <c r="B41" s="0">
         <v>2</v>
@@ -5749,22 +5696,22 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B42" s="0">
         <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>0.96599999999999997</v>
+        <v>0.96599000000000002</v>
       </c>
       <c r="D42" s="0">
         <v>0.96433000000000002</v>
       </c>
       <c r="E42" s="0">
-        <v>0.98045000000000004</v>
+        <v>0.98043999999999998</v>
       </c>
       <c r="F42" s="0">
-        <v>0.98485999999999996</v>
+        <v>0.98482999999999998</v>
       </c>
       <c r="G42" s="0">
         <v>0.96496000000000004</v>
@@ -5772,19 +5719,19 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B43" s="0">
         <v>1</v>
       </c>
       <c r="C43" s="0">
-        <v>0.02598</v>
+        <v>0.025989999999999999</v>
       </c>
       <c r="D43" s="0">
-        <v>0.02768</v>
+        <v>0.027689999999999999</v>
       </c>
       <c r="E43" s="0">
-        <v>0.016039999999999999</v>
+        <v>0.016049999999999998</v>
       </c>
       <c r="F43" s="0">
         <v>0.0135</v>
@@ -5795,13 +5742,13 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B44" s="0">
         <v>2</v>
       </c>
       <c r="C44" s="0">
-        <v>0.00564</v>
+        <v>0.0056299999999999996</v>
       </c>
       <c r="D44" s="0">
         <v>0.00611</v>
@@ -5810,7 +5757,7 @@
         <v>0.0033500000000000001</v>
       </c>
       <c r="F44" s="0">
-        <v>0.0013500000000000001</v>
+        <v>0.00139</v>
       </c>
       <c r="G44" s="0">
         <v>0</v>
@@ -5818,7 +5765,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B45" s="0">
         <v>3</v>
@@ -5841,7 +5788,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B46" s="0">
         <v>4</v>
@@ -5864,7 +5811,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B47" s="0">
         <v>5</v>
@@ -5887,7 +5834,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B48" s="0">
         <v>6</v>
@@ -5910,7 +5857,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B49" s="0">
         <v>7</v>
@@ -5933,7 +5880,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B50" s="0">
         <v>8</v>
@@ -5956,7 +5903,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B51" s="0">
         <v>9</v>
@@ -5979,7 +5926,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>338</v>
+        <v>219</v>
       </c>
       <c r="B52" s="0">
         <v>10</v>
@@ -6002,19 +5949,19 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
       </c>
       <c r="C53" s="0">
-        <v>0.96174999999999999</v>
+        <v>0.96177999999999997</v>
       </c>
       <c r="D53" s="0">
-        <v>0.97889000000000004</v>
+        <v>0.97896000000000005</v>
       </c>
       <c r="E53" s="0">
-        <v>0.98321999999999998</v>
+        <v>0.98314999999999997</v>
       </c>
       <c r="F53" s="0">
         <v>0.99999000000000005</v>
@@ -6025,7 +5972,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B54" s="0">
         <v>1</v>
@@ -6034,10 +5981,10 @@
         <v>0.031260000000000003</v>
       </c>
       <c r="D54" s="0">
-        <v>0.01617</v>
+        <v>0.016150000000000001</v>
       </c>
       <c r="E54" s="0">
-        <v>0.012189999999999999</v>
+        <v>0.01234</v>
       </c>
       <c r="F54" s="0">
         <v>0</v>
@@ -6048,7 +5995,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B55" s="0">
         <v>2</v>
@@ -6057,10 +6004,10 @@
         <v>0.0052900000000000004</v>
       </c>
       <c r="D55" s="0">
-        <v>0.00413</v>
+        <v>0.0040800000000000003</v>
       </c>
       <c r="E55" s="0">
-        <v>0.0045700000000000003</v>
+        <v>0.0044999999999999997</v>
       </c>
       <c r="F55" s="0">
         <v>0</v>
@@ -6071,7 +6018,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B56" s="0">
         <v>3</v>
@@ -6080,7 +6027,7 @@
         <v>0.00072999999999999996</v>
       </c>
       <c r="D56" s="0">
-        <v>0.00077999999999999999</v>
+        <v>0.00079000000000000001</v>
       </c>
       <c r="E56" s="0">
         <v>0</v>
@@ -6094,13 +6041,13 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B57" s="0">
         <v>4</v>
       </c>
       <c r="C57" s="0">
-        <v>5.0000000000000002e-05</v>
+        <v>3.0000000000000001e-05</v>
       </c>
       <c r="D57" s="0">
         <v>0</v>
@@ -6117,7 +6064,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B58" s="0">
         <v>5</v>
@@ -6140,7 +6087,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B59" s="0">
         <v>6</v>
@@ -6163,7 +6110,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B60" s="0">
         <v>7</v>
@@ -6186,7 +6133,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B61" s="0">
         <v>8</v>
@@ -6209,7 +6156,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B62" s="0">
         <v>9</v>
@@ -6232,7 +6179,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B63" s="0">
         <v>10</v>
@@ -6254,190 +6201,200 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.046875" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="11.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="0">
+        <v>125187.68000000001</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1208534.95</v>
+      </c>
+      <c r="D2" s="0">
+        <v>835911.09000000008</v>
+      </c>
+      <c r="E2" s="0">
+        <v>1065744.21</v>
+      </c>
+      <c r="F2" s="0">
+        <v>1146834.2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="0">
+        <v>372516.72999999998</v>
+      </c>
+      <c r="C3" s="0">
+        <v>3964294.7000000002</v>
+      </c>
+      <c r="D3" s="0">
+        <v>3293000.77</v>
+      </c>
+      <c r="E3" s="0">
+        <v>4712401.5</v>
+      </c>
+      <c r="F3" s="0">
+        <v>642754.29000000004</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="0">
+        <v>20507084.09</v>
+      </c>
+      <c r="C4" s="0">
+        <v>51286317.610000007</v>
+      </c>
+      <c r="D4" s="0">
+        <v>22797768.25</v>
+      </c>
+      <c r="E4" s="0">
+        <v>26787392.510000002</v>
+      </c>
+      <c r="F4" s="0">
+        <v>330340.22999999998</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1669454.4000000001</v>
+      </c>
+      <c r="C5" s="0">
+        <v>3830941.8199999998</v>
+      </c>
+      <c r="D5" s="0">
+        <v>3025376.4199999999</v>
+      </c>
+      <c r="E5" s="0">
+        <v>2291721.4899999998</v>
+      </c>
+      <c r="F5" s="0">
+        <v>217965.92000000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="0">
+        <v>5224649.4099999992</v>
+      </c>
+      <c r="C6" s="0">
+        <v>10273479.950000001</v>
+      </c>
+      <c r="D6" s="0">
+        <v>8887377.4600000009</v>
+      </c>
+      <c r="E6" s="0">
+        <v>10308483.369999999</v>
+      </c>
+      <c r="F6" s="0">
+        <v>700641.6399999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="0">
+        <v>13296737.390000002</v>
+      </c>
+      <c r="C7" s="0">
+        <v>14459363.270000001</v>
+      </c>
+      <c r="D7" s="0">
+        <v>4799054.7299999986</v>
+      </c>
+      <c r="E7" s="0">
+        <v>5024534.8300000001</v>
+      </c>
+      <c r="F7" s="0">
+        <v>103677.07000000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1593925.8099999998</v>
+      </c>
+      <c r="C8" s="0">
+        <v>6045459.6699999999</v>
+      </c>
+      <c r="D8" s="0">
+        <v>1637880.73</v>
+      </c>
+      <c r="E8" s="0">
+        <v>1967342.71</v>
+      </c>
+      <c r="F8" s="0">
+        <v>128836.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.046875" customWidth="true"/>
-    <col min="2" max="2" width="11.7109375" customWidth="true"/>
-    <col min="3" max="3" width="11.7109375" customWidth="true"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true"/>
-    <col min="5" max="5" width="11.7109375" customWidth="true"/>
-    <col min="6" max="6" width="9.7109375" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="B2" s="0">
-        <v>125187.68000000001</v>
-      </c>
-      <c r="C2" s="0">
-        <v>1208534.95</v>
-      </c>
-      <c r="D2" s="0">
-        <v>835911.09000000008</v>
-      </c>
-      <c r="E2" s="0">
-        <v>1065744.21</v>
-      </c>
-      <c r="F2" s="0">
-        <v>1146834.2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="B3" s="0">
-        <v>372516.72999999998</v>
-      </c>
-      <c r="C3" s="0">
-        <v>3964294.7000000002</v>
-      </c>
-      <c r="D3" s="0">
-        <v>3293000.77</v>
-      </c>
-      <c r="E3" s="0">
-        <v>4712401.5</v>
-      </c>
-      <c r="F3" s="0">
-        <v>642754.29000000004</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="B4" s="0">
-        <v>20507084.09</v>
-      </c>
-      <c r="C4" s="0">
-        <v>51286317.610000007</v>
-      </c>
-      <c r="D4" s="0">
-        <v>22797768.25</v>
-      </c>
-      <c r="E4" s="0">
-        <v>26787392.510000002</v>
-      </c>
-      <c r="F4" s="0">
-        <v>330340.22999999998</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="B5" s="0">
-        <v>1669454.4000000001</v>
-      </c>
-      <c r="C5" s="0">
-        <v>3830941.8199999998</v>
-      </c>
-      <c r="D5" s="0">
-        <v>3025376.4199999999</v>
-      </c>
-      <c r="E5" s="0">
-        <v>2291721.4899999998</v>
-      </c>
-      <c r="F5" s="0">
-        <v>217965.92000000001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="B6" s="0">
-        <v>5224649.4099999992</v>
-      </c>
-      <c r="C6" s="0">
-        <v>10273479.950000001</v>
-      </c>
-      <c r="D6" s="0">
-        <v>8887377.4600000009</v>
-      </c>
-      <c r="E6" s="0">
-        <v>10308483.369999999</v>
-      </c>
-      <c r="F6" s="0">
-        <v>700641.6399999999</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="B7" s="0">
-        <v>13296737.390000002</v>
-      </c>
-      <c r="C7" s="0">
-        <v>14459363.270000001</v>
-      </c>
-      <c r="D7" s="0">
-        <v>4799054.7299999986</v>
-      </c>
-      <c r="E7" s="0">
-        <v>5024534.8300000001</v>
-      </c>
-      <c r="F7" s="0">
-        <v>103677.07000000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="B8" s="0">
-        <v>1593925.8099999998</v>
-      </c>
-      <c r="C8" s="0">
-        <v>6045459.6699999999</v>
-      </c>
-      <c r="D8" s="0">
-        <v>1637880.73</v>
-      </c>
-      <c r="E8" s="0">
-        <v>1967342.71</v>
-      </c>
-      <c r="F8" s="0">
-        <v>128836.13</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="B6" sqref="A6:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.37890625" customWidth="true"/>
     <col min="2" max="2" width="7.26953125" customWidth="true"/>
@@ -6445,15 +6402,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>359</v>
+        <v>240</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>364</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>360</v>
+        <v>241</v>
       </c>
       <c r="B2" s="0">
         <v>0.98999999999999999</v>
@@ -6461,7 +6418,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>361</v>
+        <v>242</v>
       </c>
       <c r="B3" s="0">
         <v>140000</v>
@@ -6469,7 +6426,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>362</v>
+        <v>243</v>
       </c>
       <c r="B4" s="0">
         <v>5</v>
@@ -6477,20 +6434,13 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>363</v>
+        <v>244</v>
       </c>
       <c r="B5" s="0">
-        <v>211.32060970000001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B6" s="0">
-        <v>211.85279370000001</v>
+        <v>68.726572099999998</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>